<commit_message>
Raport na dzień 08.05.2025
</commit_message>
<xml_diff>
--- a/Raport.xlsx
+++ b/Raport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Talib\Tokyo-Garden-Restaurant\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\majer\Desktop\Tokyo-Garden-Restaurant-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{963DD355-ACDC-4F49-88C1-C39689790736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06BC3F25-2EE7-4432-836C-2948E6D4CA0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="64">
-  <si>
-    <t>Roport zaangażowania</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="73">
   <si>
     <t>Liczba członków zespołu</t>
   </si>
@@ -223,6 +220,36 @@
   </si>
   <si>
     <t>ZamowienieRepositoryTests.cs</t>
+  </si>
+  <si>
+    <t>CustomDummyTest.cs</t>
+  </si>
+  <si>
+    <t>CustomFakeTest.cs</t>
+  </si>
+  <si>
+    <t>CustomMockTest.cs</t>
+  </si>
+  <si>
+    <t>CustomSpyTest.cs</t>
+  </si>
+  <si>
+    <t>CustomStubTest.cs</t>
+  </si>
+  <si>
+    <t>MoqDummyTest.cs</t>
+  </si>
+  <si>
+    <t>MoqMockTest.cs</t>
+  </si>
+  <si>
+    <t>MoqStubTest.cs</t>
+  </si>
+  <si>
+    <t>TestyJednostkoweBLL.csproj</t>
+  </si>
+  <si>
+    <t>Raport zaangażowania</t>
   </si>
 </sst>
 </file>
@@ -311,6 +338,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -319,9 +349,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -814,14 +841,14 @@
   <dimension ref="A1:M46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="39.85546875" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" customWidth="1"/>
     <col min="4" max="5" width="12.5703125" customWidth="1"/>
     <col min="6" max="6" width="37" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="12.5703125" customWidth="1"/>
@@ -833,12 +860,12 @@
   <sheetData>
     <row r="1" spans="1:13" ht="61.5">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="23.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2">
         <v>4</v>
@@ -846,12 +873,12 @@
     </row>
     <row r="3" spans="1:13" ht="61.5">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1"/>
       <c r="D3">
         <f>SUM(D7:D1001)</f>
-        <v>125</v>
+        <v>427</v>
       </c>
       <c r="G3">
         <f>SUM(G7:G1001)</f>
@@ -868,84 +895,84 @@
     </row>
     <row r="4" spans="1:13" ht="24.95" customHeight="1">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1"/>
       <c r="D4">
         <f>($B$2*D$3)/SUM($D$3:$AK$3)</f>
-        <v>0.33692722371967654</v>
+        <v>0.95632698768197089</v>
       </c>
       <c r="G4">
         <f>($B$2*G$3)/SUM($D$3:$AK$3)</f>
-        <v>1.6954177897574123</v>
+        <v>1.4087346024636058</v>
       </c>
       <c r="J4">
         <f>($B$2*J$3)/SUM($D$3:$AK$3)</f>
-        <v>0.65498652291105119</v>
+        <v>0.54423292273236279</v>
       </c>
       <c r="M4">
         <f>($B$2*M$3)/SUM($D$3:$AK$3)</f>
-        <v>1.3126684636118597</v>
+        <v>1.0907054871220605</v>
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="7" t="s">
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7" t="s">
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
     </row>
     <row r="6" spans="1:13">
       <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
       <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
         <v>4</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>5</v>
       </c>
-      <c r="G6" t="s">
-        <v>6</v>
-      </c>
       <c r="H6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" t="s">
         <v>4</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>5</v>
       </c>
-      <c r="J6" t="s">
-        <v>6</v>
-      </c>
       <c r="K6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L6" t="s">
         <v>4</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>5</v>
-      </c>
-      <c r="M6" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -953,34 +980,34 @@
         <v>45754</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7">
         <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G7">
         <v>25</v>
       </c>
       <c r="H7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J7">
         <v>25</v>
       </c>
       <c r="K7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M7">
         <v>25</v>
@@ -991,16 +1018,16 @@
         <v>45754</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8">
         <v>100</v>
       </c>
       <c r="E8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G8">
         <v>100</v>
@@ -1009,27 +1036,36 @@
         <v>45754</v>
       </c>
       <c r="I8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J8">
         <v>100</v>
       </c>
-      <c r="K8" s="8">
+      <c r="K8" s="9">
         <v>45772</v>
       </c>
       <c r="L8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M8">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:13">
+      <c r="B9" s="9">
+        <v>45785</v>
+      </c>
+      <c r="C9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9">
+        <v>37</v>
+      </c>
       <c r="E9" s="3">
         <v>45785</v>
       </c>
       <c r="F9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G9">
         <v>13</v>
@@ -1038,403 +1074,460 @@
         <v>45770</v>
       </c>
       <c r="I9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J9">
         <v>118</v>
       </c>
-      <c r="K9" s="8"/>
+      <c r="K9" s="9"/>
       <c r="L9" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M9">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:13">
+      <c r="B10" s="9"/>
+      <c r="C10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10">
+        <v>41</v>
+      </c>
       <c r="F10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G10">
         <v>57</v>
       </c>
-      <c r="K10" s="8"/>
+      <c r="K10" s="9"/>
       <c r="L10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M10">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:13">
+      <c r="B11" s="9"/>
+      <c r="C11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11">
+        <v>43</v>
+      </c>
       <c r="F11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G11">
         <v>59</v>
       </c>
-      <c r="K11" s="8"/>
+      <c r="K11" s="9"/>
       <c r="L11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M11">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:13">
+      <c r="B12" s="9"/>
+      <c r="C12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12">
+        <v>44</v>
+      </c>
       <c r="F12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G12">
         <v>58</v>
       </c>
-      <c r="K12" s="8"/>
+      <c r="K12" s="9"/>
       <c r="L12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M12">
         <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:13">
+      <c r="B13" s="9"/>
+      <c r="C13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13">
+        <v>36</v>
+      </c>
       <c r="F13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G13">
         <v>57</v>
       </c>
-      <c r="K13" s="8"/>
+      <c r="K13" s="9"/>
       <c r="L13" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M13">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:13">
+      <c r="B14" s="9"/>
+      <c r="C14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14">
+        <v>22</v>
+      </c>
       <c r="F14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G14">
         <v>61</v>
       </c>
-      <c r="K14" s="8"/>
+      <c r="K14" s="9"/>
       <c r="L14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M14">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:13">
+      <c r="B15" s="9"/>
+      <c r="C15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15">
+        <v>23</v>
+      </c>
       <c r="F15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G15">
         <v>60</v>
       </c>
-      <c r="K15" s="8"/>
+      <c r="K15" s="9"/>
       <c r="L15" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M15">
         <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:13">
+      <c r="B16" s="9"/>
+      <c r="C16" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16">
+        <v>26</v>
+      </c>
       <c r="F16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G16">
         <v>16</v>
       </c>
-      <c r="K16" s="8"/>
+      <c r="K16" s="9"/>
       <c r="L16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M16">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="6:13">
+    <row r="17" spans="2:13">
+      <c r="B17" s="9"/>
+      <c r="C17" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17">
+        <v>30</v>
+      </c>
       <c r="F17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G17">
         <v>59</v>
       </c>
-      <c r="K17" s="8"/>
+      <c r="K17" s="9"/>
       <c r="L17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M17">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="6:13">
+    <row r="18" spans="2:13">
       <c r="F18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G18">
         <v>64</v>
       </c>
-      <c r="K18" s="8"/>
+      <c r="K18" s="9"/>
       <c r="L18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M18">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="6:13">
-      <c r="K19" s="8"/>
+    <row r="19" spans="2:13">
+      <c r="K19" s="9"/>
       <c r="L19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M19">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="6:13">
-      <c r="K20" s="8"/>
+    <row r="20" spans="2:13">
+      <c r="K20" s="9"/>
       <c r="L20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M20">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="6:13">
-      <c r="K21" s="8"/>
+    <row r="21" spans="2:13">
+      <c r="K21" s="9"/>
       <c r="L21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M21">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="6:13">
-      <c r="K22" s="8"/>
+    <row r="22" spans="2:13">
+      <c r="K22" s="9"/>
       <c r="L22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M22">
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="6:13">
-      <c r="K23" s="8"/>
+    <row r="23" spans="2:13">
+      <c r="K23" s="9"/>
       <c r="L23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M23">
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="6:13">
-      <c r="K24" s="8"/>
+    <row r="24" spans="2:13">
+      <c r="K24" s="9"/>
       <c r="L24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M24">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="6:13">
-      <c r="K25" s="8"/>
+    <row r="25" spans="2:13">
+      <c r="K25" s="9"/>
       <c r="L25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="6:13">
-      <c r="K26" s="8"/>
+    <row r="26" spans="2:13">
+      <c r="K26" s="9"/>
       <c r="L26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M26">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="6:13">
-      <c r="K27" s="8"/>
+    <row r="27" spans="2:13">
+      <c r="K27" s="9"/>
       <c r="L27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M27">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="6:13">
-      <c r="K28" s="8"/>
+    <row r="28" spans="2:13">
+      <c r="K28" s="9"/>
       <c r="L28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M28">
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="6:13">
-      <c r="K29" s="8"/>
+    <row r="29" spans="2:13">
+      <c r="K29" s="9"/>
       <c r="L29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M29">
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="6:13">
-      <c r="K30" s="8"/>
+    <row r="30" spans="2:13">
+      <c r="K30" s="9"/>
       <c r="L30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M30">
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="6:13">
-      <c r="K31" s="8"/>
+    <row r="31" spans="2:13">
+      <c r="K31" s="9"/>
       <c r="L31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M31">
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="6:13">
-      <c r="K32" s="8"/>
+    <row r="32" spans="2:13">
+      <c r="K32" s="9"/>
       <c r="L32" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M32">
         <v>11</v>
       </c>
     </row>
     <row r="33" spans="11:13">
-      <c r="K33" s="8"/>
+      <c r="K33" s="9"/>
       <c r="L33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M33">
         <v>11</v>
       </c>
     </row>
     <row r="34" spans="11:13">
-      <c r="K34" s="8"/>
+      <c r="K34" s="9"/>
       <c r="L34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M34">
         <v>11</v>
       </c>
     </row>
     <row r="35" spans="11:13">
-      <c r="K35" s="8"/>
+      <c r="K35" s="9"/>
       <c r="L35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M35">
         <v>12</v>
       </c>
     </row>
     <row r="36" spans="11:13">
-      <c r="K36" s="8"/>
+      <c r="K36" s="9"/>
       <c r="L36" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M36">
         <v>11</v>
       </c>
     </row>
     <row r="37" spans="11:13">
-      <c r="K37" s="8"/>
+      <c r="K37" s="9"/>
       <c r="L37" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M37">
         <v>3</v>
       </c>
     </row>
     <row r="38" spans="11:13">
-      <c r="K38" s="8"/>
+      <c r="K38" s="9"/>
       <c r="L38" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M38">
         <v>12</v>
       </c>
     </row>
     <row r="39" spans="11:13">
-      <c r="K39" s="8"/>
+      <c r="K39" s="9"/>
       <c r="L39" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M39">
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="11:13">
-      <c r="K40" s="8"/>
+      <c r="K40" s="9"/>
       <c r="L40" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M40">
         <v>13</v>
       </c>
     </row>
     <row r="41" spans="11:13">
-      <c r="K41" s="8"/>
+      <c r="K41" s="9"/>
       <c r="L41" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M41">
         <v>20</v>
       </c>
     </row>
     <row r="42" spans="11:13">
-      <c r="K42" s="8"/>
+      <c r="K42" s="9"/>
       <c r="L42" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M42">
         <v>16</v>
       </c>
     </row>
     <row r="43" spans="11:13">
-      <c r="K43" s="8"/>
+      <c r="K43" s="9"/>
       <c r="L43" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M43">
         <v>2</v>
       </c>
     </row>
     <row r="44" spans="11:13">
-      <c r="K44" s="8"/>
+      <c r="K44" s="9"/>
       <c r="L44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M44">
         <v>25</v>
       </c>
     </row>
     <row r="45" spans="11:13">
-      <c r="K45" s="8"/>
-      <c r="L45" s="9"/>
+      <c r="K45" s="9"/>
+      <c r="L45" s="6"/>
     </row>
     <row r="46" spans="11:13">
-      <c r="K46" s="8"/>
-      <c r="L46" s="9"/>
+      <c r="K46" s="9"/>
+      <c r="L46" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="E5:G5"/>
     <mergeCell ref="H5:J5"/>
     <mergeCell ref="K5:M5"/>
     <mergeCell ref="K8:K46"/>
+    <mergeCell ref="B9:B17"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
dodanie kontrolerów + uzupełnienie raportu
</commit_message>
<xml_diff>
--- a/Raport.xlsx
+++ b/Raport.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dominik\Downloads\Tokyo-Garden-Restaurant-main\Tokyo-Garden-Restaurant-main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dominik\source\repos\WEB_API\WEB_API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC28A72-0798-44CE-A02D-ABF2D0CA2716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A132FCB-597C-45E9-908C-B8D41949C403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
+    <sheet name="Arkusz2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="83">
   <si>
     <t>Liczba członków zespołu</t>
   </si>
@@ -253,6 +254,33 @@
   </si>
   <si>
     <t>Dodanie dodatkowych funkcji do klas</t>
+  </si>
+  <si>
+    <t>KategoriaController.cs</t>
+  </si>
+  <si>
+    <t>AdresyKontroler.cs</t>
+  </si>
+  <si>
+    <t>AlergenPozycjaMenuKontroller.cs</t>
+  </si>
+  <si>
+    <t>AlergenyKontroller.cs</t>
+  </si>
+  <si>
+    <t>PozycjeMenuController.cs</t>
+  </si>
+  <si>
+    <t>PozycjeZamowieniaController.cs</t>
+  </si>
+  <si>
+    <t>UzytkownikController.cs</t>
+  </si>
+  <si>
+    <t>ZamowieniaController.cs</t>
+  </si>
+  <si>
+    <t>Poprawienie pliku program.cs</t>
   </si>
 </sst>
 </file>
@@ -843,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
@@ -889,7 +917,7 @@
       </c>
       <c r="J3">
         <f>SUM(J7:J1001)</f>
-        <v>313</v>
+        <v>546</v>
       </c>
       <c r="M3">
         <f>SUM(M7:M1001)</f>
@@ -903,19 +931,19 @@
       <c r="B4" s="1"/>
       <c r="D4">
         <f>($B$2*D$3)/SUM($D$3:$AK$3)</f>
-        <v>0.92025862068965514</v>
+        <v>0.81761608425083776</v>
       </c>
       <c r="G4">
         <f>($B$2*G$3)/SUM($D$3:$AK$3)</f>
-        <v>1.3556034482758621</v>
+        <v>1.2044040210627094</v>
       </c>
       <c r="J4">
         <f>($B$2*J$3)/SUM($D$3:$AK$3)</f>
-        <v>0.67456896551724133</v>
+        <v>1.0454763044518909</v>
       </c>
       <c r="M4">
         <f>($B$2*M$3)/SUM($D$3:$AK$3)</f>
-        <v>1.0495689655172413</v>
+        <v>0.93250359023456197</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -1104,8 +1132,8 @@
       <c r="G10">
         <v>57</v>
       </c>
-      <c r="H10" s="3">
-        <v>45834</v>
+      <c r="H10" s="9">
+        <v>45803</v>
       </c>
       <c r="I10" t="s">
         <v>73</v>
@@ -1135,6 +1163,13 @@
       <c r="G11">
         <v>59</v>
       </c>
+      <c r="H11" s="9"/>
+      <c r="I11" t="s">
+        <v>75</v>
+      </c>
+      <c r="J11">
+        <v>23</v>
+      </c>
       <c r="K11" s="9"/>
       <c r="L11" t="s">
         <v>19</v>
@@ -1157,6 +1192,13 @@
       <c r="G12">
         <v>58</v>
       </c>
+      <c r="H12" s="9"/>
+      <c r="I12" t="s">
+        <v>77</v>
+      </c>
+      <c r="J12">
+        <v>23</v>
+      </c>
       <c r="K12" s="9"/>
       <c r="L12" t="s">
         <v>20</v>
@@ -1179,6 +1221,13 @@
       <c r="G13">
         <v>57</v>
       </c>
+      <c r="H13" s="9"/>
+      <c r="I13" t="s">
+        <v>76</v>
+      </c>
+      <c r="J13">
+        <v>27</v>
+      </c>
       <c r="K13" s="9"/>
       <c r="L13" s="5" t="s">
         <v>21</v>
@@ -1201,6 +1250,13 @@
       <c r="G14">
         <v>61</v>
       </c>
+      <c r="H14" s="9"/>
+      <c r="I14" t="s">
+        <v>74</v>
+      </c>
+      <c r="J14">
+        <v>24</v>
+      </c>
       <c r="K14" s="9"/>
       <c r="L14" t="s">
         <v>22</v>
@@ -1223,6 +1279,13 @@
       <c r="G15">
         <v>60</v>
       </c>
+      <c r="H15" s="9"/>
+      <c r="I15" t="s">
+        <v>78</v>
+      </c>
+      <c r="J15">
+        <v>27</v>
+      </c>
       <c r="K15" s="9"/>
       <c r="L15" s="5" t="s">
         <v>23</v>
@@ -1245,6 +1308,13 @@
       <c r="G16">
         <v>16</v>
       </c>
+      <c r="H16" s="9"/>
+      <c r="I16" t="s">
+        <v>79</v>
+      </c>
+      <c r="J16">
+        <v>27</v>
+      </c>
       <c r="K16" s="9"/>
       <c r="L16" t="s">
         <v>24</v>
@@ -1267,6 +1337,13 @@
       <c r="G17">
         <v>59</v>
       </c>
+      <c r="H17" s="9"/>
+      <c r="I17" t="s">
+        <v>80</v>
+      </c>
+      <c r="J17">
+        <v>27</v>
+      </c>
       <c r="K17" s="9"/>
       <c r="L17" t="s">
         <v>25</v>
@@ -1282,6 +1359,13 @@
       <c r="G18">
         <v>64</v>
       </c>
+      <c r="H18" s="9"/>
+      <c r="I18" t="s">
+        <v>81</v>
+      </c>
+      <c r="J18">
+        <v>27</v>
+      </c>
       <c r="K18" s="9"/>
       <c r="L18" t="s">
         <v>26</v>
@@ -1291,6 +1375,13 @@
       </c>
     </row>
     <row r="19" spans="2:13">
+      <c r="H19" s="9"/>
+      <c r="I19" t="s">
+        <v>82</v>
+      </c>
+      <c r="J19">
+        <v>28</v>
+      </c>
       <c r="K19" s="9"/>
       <c r="L19" t="s">
         <v>27</v>
@@ -1533,14 +1624,39 @@
       <c r="L46" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="E5:G5"/>
     <mergeCell ref="H5:J5"/>
     <mergeCell ref="K5:M5"/>
     <mergeCell ref="K8:K46"/>
     <mergeCell ref="B9:B17"/>
+    <mergeCell ref="H10:H19"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B92F9BC-6318-413C-87D9-FEE5073A822A}">
+  <dimension ref="E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="28.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="5:5">
+      <c r="E1">
+        <f>SUM(B:B)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Aktualizacja danych w raporcie
</commit_message>
<xml_diff>
--- a/Raport.xlsx
+++ b/Raport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dominik\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9142EE6E-EE3B-486E-8EF2-BE9B8A9516C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEBC64BE-6DB7-4D98-8C35-0B4C59EF72BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="293">
   <si>
     <t>Liczba członków zespołu</t>
   </si>
@@ -841,34 +841,96 @@
     <t>Dodanie kodu w pozycja-list.component.ts</t>
   </si>
   <si>
-    <t>Dodanie kodu w alergen-form.component.html</t>
-  </si>
-  <si>
-    <t>Dodanie kodu w alergen-list.component.html</t>
-  </si>
-  <si>
-    <t>Dodanie kodu w kategorie-form.component.html</t>
-  </si>
-  <si>
-    <t>Dodanie kodu w kategorie-list.component.html</t>
-  </si>
-  <si>
-    <t>Dodanie kodu w pozycja-form.component.html</t>
-  </si>
-  <si>
-    <t>Dodanie kodu w pozycja-list.component.html</t>
+    <t>Dodanie kodu w alergen-form.component.html (wyjście do panelu administratora)</t>
+  </si>
+  <si>
+    <t>Dodanie kodu w alergen-list.component.html (wyjście do panelu administratora)</t>
+  </si>
+  <si>
+    <t>Dodanie kodu w kategorie-form.component.html (wyjście do panelu administratora)</t>
+  </si>
+  <si>
+    <t>Dodanie kodu w kategorie-list.component.html (wyjście do panelu administratora)</t>
+  </si>
+  <si>
+    <t>Dodanie kodu w pozycja-form.component.html (wyjście do panelu administratora)</t>
+  </si>
+  <si>
+    <t>Dodanie kodu w pozycja-list.component.html (wyjście do panelu administratora)</t>
+  </si>
+  <si>
+    <t>menu-component.ts</t>
+  </si>
+  <si>
+    <t>menu-component.html</t>
+  </si>
+  <si>
+    <t>cart.service.ts</t>
+  </si>
+  <si>
+    <t>header.component.ts</t>
+  </si>
+  <si>
+    <t>header.component.html</t>
+  </si>
+  <si>
+    <t>cart.component.html</t>
+  </si>
+  <si>
+    <t>cart.component.ts</t>
+  </si>
+  <si>
+    <t>orders.component.html</t>
+  </si>
+  <si>
+    <t>orders.component.ts</t>
+  </si>
+  <si>
+    <t>menu.service.ts</t>
+  </si>
+  <si>
+    <t>alergen-list.component.ts:</t>
+  </si>
+  <si>
+    <t>alergen.service.ts:</t>
+  </si>
+  <si>
+    <t>kategoria-list.component.ts:</t>
+  </si>
+  <si>
+    <t>pozycja-list.component.ts:</t>
+  </si>
+  <si>
+    <t>pozycja-form.component.html</t>
+  </si>
+  <si>
+    <t>pozycja-form.component.ts</t>
+  </si>
+  <si>
+    <t>styles.css</t>
+  </si>
+  <si>
+    <t>cart.component.css</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -974,14 +1036,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -990,11 +1052,14 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -1012,17 +1077,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1514,8 +1582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M147"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G93" sqref="G93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -1560,7 +1628,7 @@
       </c>
       <c r="J3">
         <f>SUM(J7:J1001)</f>
-        <v>1280</v>
+        <v>1524</v>
       </c>
       <c r="M3">
         <f>SUM(M7:M1001)</f>
@@ -1574,42 +1642,42 @@
       <c r="B4" s="1"/>
       <c r="D4">
         <f>($B$2*D$3)/SUM($D$3:$AK$3)</f>
-        <v>0.71026490066225167</v>
+        <v>0.68713294180459161</v>
       </c>
       <c r="G4">
         <f>($B$2*G$3)/SUM($D$3:$AK$3)</f>
-        <v>0.84933774834437081</v>
+        <v>0.82167645488521091</v>
       </c>
       <c r="J4">
         <f>($B$2*J$3)/SUM($D$3:$AK$3)</f>
-        <v>0.70640176600441507</v>
+        <v>0.81366791243993597</v>
       </c>
       <c r="M4">
         <f>($B$2*M$3)/SUM($D$3:$AK$3)</f>
-        <v>1.7339955849889626</v>
+        <v>1.6775226908702616</v>
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="14" t="s">
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14" t="s">
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14" t="s">
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
     </row>
     <row r="6" spans="1:13">
       <c r="B6" t="s">
@@ -1715,7 +1783,7 @@
       <c r="J8">
         <v>100</v>
       </c>
-      <c r="K8" s="13">
+      <c r="K8" s="16">
         <v>45772</v>
       </c>
       <c r="L8" t="s">
@@ -1726,7 +1794,7 @@
       </c>
     </row>
     <row r="9" spans="1:13">
-      <c r="B9" s="13">
+      <c r="B9" s="16">
         <v>45785</v>
       </c>
       <c r="C9" t="s">
@@ -1753,7 +1821,7 @@
       <c r="J9">
         <v>118</v>
       </c>
-      <c r="K9" s="13"/>
+      <c r="K9" s="16"/>
       <c r="L9" s="5" t="s">
         <v>17</v>
       </c>
@@ -1762,7 +1830,7 @@
       </c>
     </row>
     <row r="10" spans="1:13">
-      <c r="B10" s="13"/>
+      <c r="B10" s="16"/>
       <c r="C10" t="s">
         <v>64</v>
       </c>
@@ -1775,7 +1843,7 @@
       <c r="G10">
         <v>57</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="16">
         <v>45803</v>
       </c>
       <c r="I10" t="s">
@@ -1784,7 +1852,7 @@
       <c r="J10">
         <v>70</v>
       </c>
-      <c r="K10" s="13"/>
+      <c r="K10" s="16"/>
       <c r="L10" t="s">
         <v>18</v>
       </c>
@@ -1793,7 +1861,7 @@
       </c>
     </row>
     <row r="11" spans="1:13">
-      <c r="B11" s="13"/>
+      <c r="B11" s="16"/>
       <c r="C11" t="s">
         <v>65</v>
       </c>
@@ -1806,14 +1874,14 @@
       <c r="G11">
         <v>59</v>
       </c>
-      <c r="H11" s="13"/>
+      <c r="H11" s="16"/>
       <c r="I11" t="s">
         <v>75</v>
       </c>
       <c r="J11">
         <v>23</v>
       </c>
-      <c r="K11" s="13"/>
+      <c r="K11" s="16"/>
       <c r="L11" t="s">
         <v>19</v>
       </c>
@@ -1822,7 +1890,7 @@
       </c>
     </row>
     <row r="12" spans="1:13">
-      <c r="B12" s="13"/>
+      <c r="B12" s="16"/>
       <c r="C12" t="s">
         <v>66</v>
       </c>
@@ -1835,14 +1903,14 @@
       <c r="G12">
         <v>58</v>
       </c>
-      <c r="H12" s="13"/>
+      <c r="H12" s="16"/>
       <c r="I12" t="s">
         <v>77</v>
       </c>
       <c r="J12">
         <v>23</v>
       </c>
-      <c r="K12" s="13"/>
+      <c r="K12" s="16"/>
       <c r="L12" t="s">
         <v>20</v>
       </c>
@@ -1851,7 +1919,7 @@
       </c>
     </row>
     <row r="13" spans="1:13">
-      <c r="B13" s="13"/>
+      <c r="B13" s="16"/>
       <c r="C13" t="s">
         <v>67</v>
       </c>
@@ -1864,14 +1932,14 @@
       <c r="G13">
         <v>57</v>
       </c>
-      <c r="H13" s="13"/>
+      <c r="H13" s="16"/>
       <c r="I13" t="s">
         <v>76</v>
       </c>
       <c r="J13">
         <v>27</v>
       </c>
-      <c r="K13" s="13"/>
+      <c r="K13" s="16"/>
       <c r="L13" s="5" t="s">
         <v>21</v>
       </c>
@@ -1880,7 +1948,7 @@
       </c>
     </row>
     <row r="14" spans="1:13">
-      <c r="B14" s="13"/>
+      <c r="B14" s="16"/>
       <c r="C14" t="s">
         <v>68</v>
       </c>
@@ -1893,14 +1961,14 @@
       <c r="G14">
         <v>61</v>
       </c>
-      <c r="H14" s="13"/>
+      <c r="H14" s="16"/>
       <c r="I14" t="s">
         <v>74</v>
       </c>
       <c r="J14">
         <v>24</v>
       </c>
-      <c r="K14" s="13"/>
+      <c r="K14" s="16"/>
       <c r="L14" t="s">
         <v>22</v>
       </c>
@@ -1909,7 +1977,7 @@
       </c>
     </row>
     <row r="15" spans="1:13">
-      <c r="B15" s="13"/>
+      <c r="B15" s="16"/>
       <c r="C15" t="s">
         <v>69</v>
       </c>
@@ -1922,14 +1990,14 @@
       <c r="G15">
         <v>60</v>
       </c>
-      <c r="H15" s="13"/>
+      <c r="H15" s="16"/>
       <c r="I15" t="s">
         <v>78</v>
       </c>
       <c r="J15">
         <v>27</v>
       </c>
-      <c r="K15" s="13"/>
+      <c r="K15" s="16"/>
       <c r="L15" s="5" t="s">
         <v>23</v>
       </c>
@@ -1938,7 +2006,7 @@
       </c>
     </row>
     <row r="16" spans="1:13">
-      <c r="B16" s="13"/>
+      <c r="B16" s="16"/>
       <c r="C16" t="s">
         <v>70</v>
       </c>
@@ -1951,14 +2019,14 @@
       <c r="G16">
         <v>16</v>
       </c>
-      <c r="H16" s="13"/>
+      <c r="H16" s="16"/>
       <c r="I16" t="s">
         <v>79</v>
       </c>
       <c r="J16">
         <v>27</v>
       </c>
-      <c r="K16" s="13"/>
+      <c r="K16" s="16"/>
       <c r="L16" t="s">
         <v>24</v>
       </c>
@@ -1967,7 +2035,7 @@
       </c>
     </row>
     <row r="17" spans="2:13">
-      <c r="B17" s="13"/>
+      <c r="B17" s="16"/>
       <c r="C17" t="s">
         <v>71</v>
       </c>
@@ -1980,14 +2048,14 @@
       <c r="G17">
         <v>59</v>
       </c>
-      <c r="H17" s="13"/>
+      <c r="H17" s="16"/>
       <c r="I17" t="s">
         <v>80</v>
       </c>
       <c r="J17">
         <v>27</v>
       </c>
-      <c r="K17" s="13"/>
+      <c r="K17" s="16"/>
       <c r="L17" t="s">
         <v>25</v>
       </c>
@@ -1996,7 +2064,7 @@
       </c>
     </row>
     <row r="18" spans="2:13">
-      <c r="B18" s="13">
+      <c r="B18" s="16">
         <v>45803</v>
       </c>
       <c r="C18" t="s">
@@ -2011,14 +2079,14 @@
       <c r="G18">
         <v>64</v>
       </c>
-      <c r="H18" s="13"/>
+      <c r="H18" s="16"/>
       <c r="I18" t="s">
         <v>81</v>
       </c>
       <c r="J18">
         <v>27</v>
       </c>
-      <c r="K18" s="13"/>
+      <c r="K18" s="16"/>
       <c r="L18" t="s">
         <v>26</v>
       </c>
@@ -2027,21 +2095,21 @@
       </c>
     </row>
     <row r="19" spans="2:13">
-      <c r="B19" s="13"/>
+      <c r="B19" s="16"/>
       <c r="C19" t="s">
         <v>85</v>
       </c>
       <c r="D19">
         <v>144</v>
       </c>
-      <c r="H19" s="13"/>
+      <c r="H19" s="16"/>
       <c r="I19" t="s">
         <v>82</v>
       </c>
       <c r="J19">
         <v>28</v>
       </c>
-      <c r="K19" s="13"/>
+      <c r="K19" s="16"/>
       <c r="L19" t="s">
         <v>27</v>
       </c>
@@ -2050,21 +2118,21 @@
       </c>
     </row>
     <row r="20" spans="2:13">
-      <c r="B20" s="13"/>
+      <c r="B20" s="16"/>
       <c r="C20" t="s">
         <v>86</v>
       </c>
       <c r="D20">
         <v>164</v>
       </c>
-      <c r="H20" s="13"/>
+      <c r="H20" s="16"/>
       <c r="I20" t="s">
         <v>83</v>
       </c>
       <c r="J20">
         <v>34</v>
       </c>
-      <c r="K20" s="13"/>
+      <c r="K20" s="16"/>
       <c r="L20" t="s">
         <v>28</v>
       </c>
@@ -2073,14 +2141,14 @@
       </c>
     </row>
     <row r="21" spans="2:13">
-      <c r="B21" s="13"/>
+      <c r="B21" s="16"/>
       <c r="C21" t="s">
         <v>87</v>
       </c>
       <c r="D21">
         <v>58</v>
       </c>
-      <c r="E21" s="13">
+      <c r="E21" s="16">
         <v>45804</v>
       </c>
       <c r="F21" t="s">
@@ -2089,7 +2157,7 @@
       <c r="G21">
         <v>81</v>
       </c>
-      <c r="H21" s="13">
+      <c r="H21" s="16">
         <v>45817</v>
       </c>
       <c r="I21" s="12" t="s">
@@ -2098,7 +2166,7 @@
       <c r="J21" s="6">
         <v>3</v>
       </c>
-      <c r="K21" s="13"/>
+      <c r="K21" s="16"/>
       <c r="L21" t="s">
         <v>29</v>
       </c>
@@ -2107,28 +2175,28 @@
       </c>
     </row>
     <row r="22" spans="2:13">
-      <c r="B22" s="13"/>
+      <c r="B22" s="16"/>
       <c r="C22" t="s">
         <v>88</v>
       </c>
       <c r="D22">
         <v>92</v>
       </c>
-      <c r="E22" s="14"/>
+      <c r="E22" s="15"/>
       <c r="F22" t="s">
         <v>102</v>
       </c>
       <c r="G22">
         <v>69</v>
       </c>
-      <c r="H22" s="13"/>
+      <c r="H22" s="16"/>
       <c r="I22" t="s">
         <v>111</v>
       </c>
       <c r="J22" s="6">
         <v>6</v>
       </c>
-      <c r="K22" s="13"/>
+      <c r="K22" s="16"/>
       <c r="L22" t="s">
         <v>30</v>
       </c>
@@ -2137,28 +2205,28 @@
       </c>
     </row>
     <row r="23" spans="2:13">
-      <c r="B23" s="13"/>
+      <c r="B23" s="16"/>
       <c r="C23" t="s">
         <v>89</v>
       </c>
       <c r="D23">
         <v>64</v>
       </c>
-      <c r="E23" s="14"/>
+      <c r="E23" s="15"/>
       <c r="F23" t="s">
         <v>103</v>
       </c>
       <c r="G23">
         <v>75</v>
       </c>
-      <c r="H23" s="13"/>
+      <c r="H23" s="16"/>
       <c r="I23" t="s">
         <v>112</v>
       </c>
       <c r="J23" s="6">
         <v>3</v>
       </c>
-      <c r="K23" s="13"/>
+      <c r="K23" s="16"/>
       <c r="L23" t="s">
         <v>31</v>
       </c>
@@ -2167,28 +2235,28 @@
       </c>
     </row>
     <row r="24" spans="2:13">
-      <c r="B24" s="13"/>
+      <c r="B24" s="16"/>
       <c r="C24" t="s">
         <v>90</v>
       </c>
       <c r="D24">
         <v>20</v>
       </c>
-      <c r="E24" s="14"/>
+      <c r="E24" s="15"/>
       <c r="F24" t="s">
         <v>104</v>
       </c>
       <c r="G24">
         <v>126</v>
       </c>
-      <c r="H24" s="13"/>
+      <c r="H24" s="16"/>
       <c r="I24" t="s">
         <v>113</v>
       </c>
       <c r="J24" s="6">
         <v>6</v>
       </c>
-      <c r="K24" s="13"/>
+      <c r="K24" s="16"/>
       <c r="L24" t="s">
         <v>32</v>
       </c>
@@ -2197,28 +2265,28 @@
       </c>
     </row>
     <row r="25" spans="2:13">
-      <c r="B25" s="13"/>
+      <c r="B25" s="16"/>
       <c r="C25" t="s">
         <v>91</v>
       </c>
       <c r="D25">
         <v>57</v>
       </c>
-      <c r="E25" s="14"/>
+      <c r="E25" s="15"/>
       <c r="F25" t="s">
         <v>105</v>
       </c>
       <c r="G25">
         <v>65</v>
       </c>
-      <c r="H25" s="13"/>
+      <c r="H25" s="16"/>
       <c r="I25" t="s">
         <v>114</v>
       </c>
       <c r="J25" s="6">
         <v>4</v>
       </c>
-      <c r="K25" s="13"/>
+      <c r="K25" s="16"/>
       <c r="L25" t="s">
         <v>33</v>
       </c>
@@ -2227,28 +2295,28 @@
       </c>
     </row>
     <row r="26" spans="2:13">
-      <c r="B26" s="13"/>
+      <c r="B26" s="16"/>
       <c r="C26" t="s">
         <v>92</v>
       </c>
       <c r="D26">
         <v>28</v>
       </c>
-      <c r="E26" s="14"/>
+      <c r="E26" s="15"/>
       <c r="F26" t="s">
         <v>106</v>
       </c>
       <c r="G26">
         <v>82</v>
       </c>
-      <c r="H26" s="13"/>
+      <c r="H26" s="16"/>
       <c r="I26" s="12" t="s">
         <v>115</v>
       </c>
       <c r="J26" s="6">
         <v>2</v>
       </c>
-      <c r="K26" s="13"/>
+      <c r="K26" s="16"/>
       <c r="L26" t="s">
         <v>34</v>
       </c>
@@ -2257,28 +2325,28 @@
       </c>
     </row>
     <row r="27" spans="2:13">
-      <c r="B27" s="13"/>
+      <c r="B27" s="16"/>
       <c r="C27" t="s">
         <v>93</v>
       </c>
       <c r="D27">
         <v>26</v>
       </c>
-      <c r="E27" s="14"/>
+      <c r="E27" s="15"/>
       <c r="F27" t="s">
         <v>107</v>
       </c>
       <c r="G27">
         <v>75</v>
       </c>
-      <c r="H27" s="13"/>
+      <c r="H27" s="16"/>
       <c r="I27" t="s">
         <v>116</v>
       </c>
       <c r="J27" s="6">
         <v>8</v>
       </c>
-      <c r="K27" s="13"/>
+      <c r="K27" s="16"/>
       <c r="L27" t="s">
         <v>35</v>
       </c>
@@ -2287,28 +2355,28 @@
       </c>
     </row>
     <row r="28" spans="2:13">
-      <c r="B28" s="13"/>
+      <c r="B28" s="16"/>
       <c r="C28" t="s">
         <v>94</v>
       </c>
       <c r="D28">
         <v>16</v>
       </c>
-      <c r="E28" s="14"/>
+      <c r="E28" s="15"/>
       <c r="F28" t="s">
         <v>108</v>
       </c>
       <c r="G28">
         <v>266</v>
       </c>
-      <c r="H28" s="13"/>
+      <c r="H28" s="16"/>
       <c r="I28" t="s">
         <v>117</v>
       </c>
       <c r="J28" s="6">
         <v>3</v>
       </c>
-      <c r="K28" s="13"/>
+      <c r="K28" s="16"/>
       <c r="L28" t="s">
         <v>36</v>
       </c>
@@ -2317,28 +2385,28 @@
       </c>
     </row>
     <row r="29" spans="2:13">
-      <c r="B29" s="13"/>
+      <c r="B29" s="16"/>
       <c r="C29" t="s">
         <v>95</v>
       </c>
       <c r="D29">
         <v>18</v>
       </c>
-      <c r="E29" s="14"/>
+      <c r="E29" s="15"/>
       <c r="F29" t="s">
         <v>109</v>
       </c>
       <c r="G29">
         <v>71</v>
       </c>
-      <c r="H29" s="13"/>
+      <c r="H29" s="16"/>
       <c r="I29" t="s">
         <v>118</v>
       </c>
       <c r="J29" s="6">
         <v>12</v>
       </c>
-      <c r="K29" s="13"/>
+      <c r="K29" s="16"/>
       <c r="L29" t="s">
         <v>37</v>
       </c>
@@ -2347,21 +2415,21 @@
       </c>
     </row>
     <row r="30" spans="2:13">
-      <c r="B30" s="13"/>
+      <c r="B30" s="16"/>
       <c r="C30" t="s">
         <v>96</v>
       </c>
       <c r="D30">
         <v>15</v>
       </c>
-      <c r="H30" s="13"/>
+      <c r="H30" s="16"/>
       <c r="I30" t="s">
         <v>119</v>
       </c>
       <c r="J30" s="6">
         <v>3</v>
       </c>
-      <c r="K30" s="13"/>
+      <c r="K30" s="16"/>
       <c r="L30" t="s">
         <v>38</v>
       </c>
@@ -2370,21 +2438,21 @@
       </c>
     </row>
     <row r="31" spans="2:13">
-      <c r="B31" s="13"/>
+      <c r="B31" s="16"/>
       <c r="C31" t="s">
         <v>97</v>
       </c>
       <c r="D31">
         <v>17</v>
       </c>
-      <c r="H31" s="13"/>
+      <c r="H31" s="16"/>
       <c r="I31" t="s">
         <v>120</v>
       </c>
       <c r="J31" s="6">
         <v>6</v>
       </c>
-      <c r="K31" s="13"/>
+      <c r="K31" s="16"/>
       <c r="L31" t="s">
         <v>39</v>
       </c>
@@ -2393,21 +2461,21 @@
       </c>
     </row>
     <row r="32" spans="2:13">
-      <c r="B32" s="13"/>
+      <c r="B32" s="16"/>
       <c r="C32" t="s">
         <v>98</v>
       </c>
       <c r="D32">
         <v>44</v>
       </c>
-      <c r="H32" s="13"/>
+      <c r="H32" s="16"/>
       <c r="I32" t="s">
         <v>121</v>
       </c>
       <c r="J32" s="6">
         <v>2</v>
       </c>
-      <c r="K32" s="13"/>
+      <c r="K32" s="16"/>
       <c r="L32" s="5" t="s">
         <v>40</v>
       </c>
@@ -2416,21 +2484,21 @@
       </c>
     </row>
     <row r="33" spans="2:13">
-      <c r="B33" s="13"/>
+      <c r="B33" s="16"/>
       <c r="C33" t="s">
         <v>99</v>
       </c>
       <c r="D33">
         <v>43</v>
       </c>
-      <c r="H33" s="13"/>
+      <c r="H33" s="16"/>
       <c r="I33" t="s">
         <v>122</v>
       </c>
       <c r="J33" s="6">
         <v>4</v>
       </c>
-      <c r="K33" s="13"/>
+      <c r="K33" s="16"/>
       <c r="L33" t="s">
         <v>41</v>
       </c>
@@ -2439,21 +2507,21 @@
       </c>
     </row>
     <row r="34" spans="2:13">
-      <c r="B34" s="13"/>
+      <c r="B34" s="16"/>
       <c r="C34" t="s">
         <v>100</v>
       </c>
       <c r="D34">
         <v>28</v>
       </c>
-      <c r="H34" s="13"/>
+      <c r="H34" s="16"/>
       <c r="I34" t="s">
         <v>123</v>
       </c>
       <c r="J34" s="6">
         <v>8</v>
       </c>
-      <c r="K34" s="13"/>
+      <c r="K34" s="16"/>
       <c r="L34" t="s">
         <v>42</v>
       </c>
@@ -2462,7 +2530,7 @@
       </c>
     </row>
     <row r="35" spans="2:13">
-      <c r="H35" s="13">
+      <c r="H35" s="16">
         <v>45898</v>
       </c>
       <c r="I35" s="9" t="s">
@@ -2471,7 +2539,7 @@
       <c r="J35" s="6">
         <v>5</v>
       </c>
-      <c r="K35" s="13"/>
+      <c r="K35" s="16"/>
       <c r="L35" t="s">
         <v>43</v>
       </c>
@@ -2480,14 +2548,14 @@
       </c>
     </row>
     <row r="36" spans="2:13">
-      <c r="H36" s="14"/>
+      <c r="H36" s="15"/>
       <c r="I36" s="9" t="s">
         <v>228</v>
       </c>
       <c r="J36" s="6">
         <v>15</v>
       </c>
-      <c r="K36" s="13"/>
+      <c r="K36" s="16"/>
       <c r="L36" t="s">
         <v>44</v>
       </c>
@@ -2496,7 +2564,7 @@
       </c>
     </row>
     <row r="37" spans="2:13">
-      <c r="H37" s="13">
+      <c r="H37" s="16">
         <v>45899</v>
       </c>
       <c r="I37" s="10" t="s">
@@ -2505,7 +2573,7 @@
       <c r="J37" s="6">
         <v>18</v>
       </c>
-      <c r="K37" s="13"/>
+      <c r="K37" s="16"/>
       <c r="L37" t="s">
         <v>45</v>
       </c>
@@ -2514,14 +2582,14 @@
       </c>
     </row>
     <row r="38" spans="2:13">
-      <c r="H38" s="13"/>
+      <c r="H38" s="16"/>
       <c r="I38" s="10" t="s">
         <v>230</v>
       </c>
       <c r="J38" s="6">
         <v>8</v>
       </c>
-      <c r="K38" s="13"/>
+      <c r="K38" s="16"/>
       <c r="L38" t="s">
         <v>46</v>
       </c>
@@ -2530,14 +2598,14 @@
       </c>
     </row>
     <row r="39" spans="2:13">
-      <c r="H39" s="13"/>
+      <c r="H39" s="16"/>
       <c r="I39" s="10" t="s">
         <v>231</v>
       </c>
       <c r="J39" s="6">
         <v>8</v>
       </c>
-      <c r="K39" s="13"/>
+      <c r="K39" s="16"/>
       <c r="L39" t="s">
         <v>47</v>
       </c>
@@ -2546,14 +2614,14 @@
       </c>
     </row>
     <row r="40" spans="2:13">
-      <c r="H40" s="13"/>
+      <c r="H40" s="16"/>
       <c r="I40" s="10" t="s">
         <v>232</v>
       </c>
       <c r="J40" s="6">
         <v>8</v>
       </c>
-      <c r="K40" s="13"/>
+      <c r="K40" s="16"/>
       <c r="L40" s="5" t="s">
         <v>48</v>
       </c>
@@ -2562,14 +2630,14 @@
       </c>
     </row>
     <row r="41" spans="2:13">
-      <c r="H41" s="13"/>
+      <c r="H41" s="16"/>
       <c r="I41" s="10" t="s">
         <v>233</v>
       </c>
       <c r="J41" s="6">
         <v>10</v>
       </c>
-      <c r="K41" s="13"/>
+      <c r="K41" s="16"/>
       <c r="L41" s="5" t="s">
         <v>49</v>
       </c>
@@ -2578,14 +2646,14 @@
       </c>
     </row>
     <row r="42" spans="2:13">
-      <c r="H42" s="13"/>
+      <c r="H42" s="16"/>
       <c r="I42" s="10" t="s">
         <v>234</v>
       </c>
       <c r="J42" s="6">
         <v>8</v>
       </c>
-      <c r="K42" s="13"/>
+      <c r="K42" s="16"/>
       <c r="L42" t="s">
         <v>50</v>
       </c>
@@ -2594,14 +2662,14 @@
       </c>
     </row>
     <row r="43" spans="2:13">
-      <c r="H43" s="13"/>
+      <c r="H43" s="16"/>
       <c r="I43" s="10" t="s">
         <v>235</v>
       </c>
       <c r="J43" s="6">
         <v>10</v>
       </c>
-      <c r="K43" s="13"/>
+      <c r="K43" s="16"/>
       <c r="L43" t="s">
         <v>51</v>
       </c>
@@ -2610,14 +2678,14 @@
       </c>
     </row>
     <row r="44" spans="2:13">
-      <c r="H44" s="13"/>
+      <c r="H44" s="16"/>
       <c r="I44" s="10" t="s">
         <v>236</v>
       </c>
       <c r="J44" s="6">
         <v>8</v>
       </c>
-      <c r="K44" s="13"/>
+      <c r="K44" s="16"/>
       <c r="L44" t="s">
         <v>52</v>
       </c>
@@ -2626,14 +2694,14 @@
       </c>
     </row>
     <row r="45" spans="2:13">
-      <c r="H45" s="13"/>
+      <c r="H45" s="16"/>
       <c r="I45" s="11" t="s">
         <v>237</v>
       </c>
       <c r="J45" s="6">
         <v>21</v>
       </c>
-      <c r="K45" s="13">
+      <c r="K45" s="16">
         <v>45898</v>
       </c>
       <c r="L45" s="7" t="s">
@@ -2644,14 +2712,14 @@
       </c>
     </row>
     <row r="46" spans="2:13">
-      <c r="H46" s="13"/>
+      <c r="H46" s="16"/>
       <c r="I46" s="11" t="s">
         <v>238</v>
       </c>
       <c r="J46" s="6">
         <v>17</v>
       </c>
-      <c r="K46" s="13"/>
+      <c r="K46" s="16"/>
       <c r="L46" s="7" t="s">
         <v>125</v>
       </c>
@@ -2660,14 +2728,14 @@
       </c>
     </row>
     <row r="47" spans="2:13">
-      <c r="H47" s="13"/>
+      <c r="H47" s="16"/>
       <c r="I47" s="11" t="s">
         <v>239</v>
       </c>
       <c r="J47" s="6">
         <v>12</v>
       </c>
-      <c r="K47" s="13"/>
+      <c r="K47" s="16"/>
       <c r="L47" t="s">
         <v>126</v>
       </c>
@@ -2676,14 +2744,14 @@
       </c>
     </row>
     <row r="48" spans="2:13">
-      <c r="H48" s="13"/>
+      <c r="H48" s="16"/>
       <c r="I48" s="11" t="s">
         <v>240</v>
       </c>
       <c r="J48" s="6">
         <v>7</v>
       </c>
-      <c r="K48" s="13"/>
+      <c r="K48" s="16"/>
       <c r="L48" t="s">
         <v>127</v>
       </c>
@@ -2692,14 +2760,14 @@
       </c>
     </row>
     <row r="49" spans="8:13">
-      <c r="H49" s="13"/>
+      <c r="H49" s="16"/>
       <c r="I49" s="11" t="s">
         <v>241</v>
       </c>
       <c r="J49" s="6">
         <v>12</v>
       </c>
-      <c r="K49" s="13"/>
+      <c r="K49" s="16"/>
       <c r="L49" t="s">
         <v>128</v>
       </c>
@@ -2708,14 +2776,14 @@
       </c>
     </row>
     <row r="50" spans="8:13">
-      <c r="H50" s="13"/>
+      <c r="H50" s="16"/>
       <c r="I50" s="11" t="s">
         <v>242</v>
       </c>
       <c r="J50" s="6">
         <v>13</v>
       </c>
-      <c r="K50" s="13"/>
+      <c r="K50" s="16"/>
       <c r="L50" t="s">
         <v>129</v>
       </c>
@@ -2724,14 +2792,14 @@
       </c>
     </row>
     <row r="51" spans="8:13">
-      <c r="H51" s="13"/>
+      <c r="H51" s="16"/>
       <c r="I51" s="11" t="s">
         <v>243</v>
       </c>
       <c r="J51" s="6">
         <v>14</v>
       </c>
-      <c r="K51" s="13"/>
+      <c r="K51" s="16"/>
       <c r="L51" t="s">
         <v>130</v>
       </c>
@@ -2740,14 +2808,14 @@
       </c>
     </row>
     <row r="52" spans="8:13">
-      <c r="H52" s="13"/>
+      <c r="H52" s="16"/>
       <c r="I52" s="11" t="s">
         <v>244</v>
       </c>
       <c r="J52" s="6">
         <v>14</v>
       </c>
-      <c r="K52" s="13"/>
+      <c r="K52" s="16"/>
       <c r="L52" t="s">
         <v>131</v>
       </c>
@@ -2756,14 +2824,14 @@
       </c>
     </row>
     <row r="53" spans="8:13">
-      <c r="H53" s="13"/>
+      <c r="H53" s="16"/>
       <c r="I53" s="11" t="s">
         <v>245</v>
       </c>
       <c r="J53" s="11">
         <v>8</v>
       </c>
-      <c r="K53" s="13"/>
+      <c r="K53" s="16"/>
       <c r="L53" s="8" t="s">
         <v>132</v>
       </c>
@@ -2772,14 +2840,14 @@
       </c>
     </row>
     <row r="54" spans="8:13">
-      <c r="H54" s="13"/>
+      <c r="H54" s="16"/>
       <c r="I54" s="11" t="s">
         <v>246</v>
       </c>
       <c r="J54" s="6">
         <v>10</v>
       </c>
-      <c r="K54" s="13"/>
+      <c r="K54" s="16"/>
       <c r="L54" t="s">
         <v>133</v>
       </c>
@@ -2788,7 +2856,7 @@
       </c>
     </row>
     <row r="55" spans="8:13">
-      <c r="H55" s="13">
+      <c r="H55" s="16">
         <v>45900</v>
       </c>
       <c r="I55" s="12" t="s">
@@ -2797,7 +2865,7 @@
       <c r="J55" s="6">
         <v>44</v>
       </c>
-      <c r="K55" s="13"/>
+      <c r="K55" s="16"/>
       <c r="L55" t="s">
         <v>134</v>
       </c>
@@ -2806,14 +2874,14 @@
       </c>
     </row>
     <row r="56" spans="8:13">
-      <c r="H56" s="13"/>
+      <c r="H56" s="16"/>
       <c r="I56" s="12" t="s">
         <v>253</v>
       </c>
       <c r="J56" s="6">
         <v>1</v>
       </c>
-      <c r="K56" s="13"/>
+      <c r="K56" s="16"/>
       <c r="L56" t="s">
         <v>135</v>
       </c>
@@ -2822,14 +2890,14 @@
       </c>
     </row>
     <row r="57" spans="8:13">
-      <c r="H57" s="13"/>
+      <c r="H57" s="16"/>
       <c r="I57" s="12" t="s">
         <v>254</v>
       </c>
       <c r="J57" s="12">
         <v>15</v>
       </c>
-      <c r="K57" s="13"/>
+      <c r="K57" s="16"/>
       <c r="L57" t="s">
         <v>136</v>
       </c>
@@ -2838,14 +2906,14 @@
       </c>
     </row>
     <row r="58" spans="8:13">
-      <c r="H58" s="13"/>
+      <c r="H58" s="16"/>
       <c r="I58" s="12" t="s">
         <v>247</v>
       </c>
       <c r="J58" s="12">
         <v>35</v>
       </c>
-      <c r="K58" s="13"/>
+      <c r="K58" s="16"/>
       <c r="L58" t="s">
         <v>137</v>
       </c>
@@ -2854,14 +2922,14 @@
       </c>
     </row>
     <row r="59" spans="8:13">
-      <c r="H59" s="13"/>
+      <c r="H59" s="16"/>
       <c r="I59" s="12" t="s">
         <v>256</v>
       </c>
       <c r="J59" s="6">
         <v>1</v>
       </c>
-      <c r="K59" s="13"/>
+      <c r="K59" s="16"/>
       <c r="L59" t="s">
         <v>138</v>
       </c>
@@ -2870,14 +2938,14 @@
       </c>
     </row>
     <row r="60" spans="8:13">
-      <c r="H60" s="13"/>
+      <c r="H60" s="16"/>
       <c r="I60" s="12" t="s">
         <v>257</v>
       </c>
       <c r="J60" s="6">
         <v>12</v>
       </c>
-      <c r="K60" s="13"/>
+      <c r="K60" s="16"/>
       <c r="L60" t="s">
         <v>139</v>
       </c>
@@ -2886,14 +2954,14 @@
       </c>
     </row>
     <row r="61" spans="8:13">
-      <c r="H61" s="13"/>
+      <c r="H61" s="16"/>
       <c r="I61" s="12" t="s">
         <v>259</v>
       </c>
       <c r="J61" s="6">
         <v>5</v>
       </c>
-      <c r="K61" s="13"/>
+      <c r="K61" s="16"/>
       <c r="L61" t="s">
         <v>140</v>
       </c>
@@ -2902,14 +2970,14 @@
       </c>
     </row>
     <row r="62" spans="8:13">
-      <c r="H62" s="13"/>
+      <c r="H62" s="16"/>
       <c r="I62" s="12" t="s">
         <v>258</v>
       </c>
       <c r="J62" s="12">
         <v>51</v>
       </c>
-      <c r="K62" s="13"/>
+      <c r="K62" s="16"/>
       <c r="L62" t="s">
         <v>141</v>
       </c>
@@ -2918,14 +2986,14 @@
       </c>
     </row>
     <row r="63" spans="8:13">
-      <c r="H63" s="13"/>
+      <c r="H63" s="16"/>
       <c r="I63" s="12" t="s">
         <v>260</v>
       </c>
       <c r="J63" s="12">
         <v>35</v>
       </c>
-      <c r="K63" s="13"/>
+      <c r="K63" s="16"/>
       <c r="L63" t="s">
         <v>142</v>
       </c>
@@ -2934,14 +3002,14 @@
       </c>
     </row>
     <row r="64" spans="8:13">
-      <c r="H64" s="13"/>
+      <c r="H64" s="16"/>
       <c r="I64" s="12" t="s">
         <v>261</v>
       </c>
       <c r="J64" s="6">
         <v>28</v>
       </c>
-      <c r="K64" s="13"/>
+      <c r="K64" s="16"/>
       <c r="L64" t="s">
         <v>143</v>
       </c>
@@ -2950,14 +3018,14 @@
       </c>
     </row>
     <row r="65" spans="8:13">
-      <c r="H65" s="13"/>
+      <c r="H65" s="16"/>
       <c r="I65" s="12" t="s">
         <v>262</v>
       </c>
       <c r="J65" s="6">
         <v>1</v>
       </c>
-      <c r="K65" s="13"/>
+      <c r="K65" s="16"/>
       <c r="L65" t="s">
         <v>144</v>
       </c>
@@ -2966,16 +3034,16 @@
       </c>
     </row>
     <row r="66" spans="8:13">
-      <c r="H66" s="13">
+      <c r="H66" s="16">
         <v>45901</v>
       </c>
-      <c r="I66" s="16" t="s">
+      <c r="I66" s="13" t="s">
         <v>263</v>
       </c>
       <c r="J66" s="6">
         <v>24</v>
       </c>
-      <c r="K66" s="13"/>
+      <c r="K66" s="16"/>
       <c r="L66" t="s">
         <v>145</v>
       </c>
@@ -2984,14 +3052,14 @@
       </c>
     </row>
     <row r="67" spans="8:13">
-      <c r="H67" s="13"/>
-      <c r="I67" s="16" t="s">
+      <c r="H67" s="16"/>
+      <c r="I67" s="13" t="s">
         <v>264</v>
       </c>
       <c r="J67" s="6">
         <v>24</v>
       </c>
-      <c r="K67" s="13"/>
+      <c r="K67" s="16"/>
       <c r="L67" t="s">
         <v>146</v>
       </c>
@@ -3000,14 +3068,14 @@
       </c>
     </row>
     <row r="68" spans="8:13">
-      <c r="H68" s="13"/>
-      <c r="I68" s="16" t="s">
+      <c r="H68" s="16"/>
+      <c r="I68" s="13" t="s">
         <v>265</v>
       </c>
       <c r="J68" s="6">
         <v>34</v>
       </c>
-      <c r="K68" s="13"/>
+      <c r="K68" s="16"/>
       <c r="L68" t="s">
         <v>147</v>
       </c>
@@ -3016,14 +3084,14 @@
       </c>
     </row>
     <row r="69" spans="8:13">
-      <c r="H69" s="13"/>
-      <c r="I69" s="16" t="s">
+      <c r="H69" s="16"/>
+      <c r="I69" s="13" t="s">
         <v>266</v>
       </c>
       <c r="J69" s="6">
         <v>33</v>
       </c>
-      <c r="K69" s="13"/>
+      <c r="K69" s="16"/>
       <c r="L69" t="s">
         <v>148</v>
       </c>
@@ -3032,14 +3100,14 @@
       </c>
     </row>
     <row r="70" spans="8:13">
-      <c r="H70" s="13"/>
-      <c r="I70" s="16" t="s">
+      <c r="H70" s="16"/>
+      <c r="I70" s="13" t="s">
         <v>267</v>
       </c>
       <c r="J70" s="6">
         <v>45</v>
       </c>
-      <c r="K70" s="13"/>
+      <c r="K70" s="16"/>
       <c r="L70" t="s">
         <v>149</v>
       </c>
@@ -3048,14 +3116,14 @@
       </c>
     </row>
     <row r="71" spans="8:13">
-      <c r="H71" s="13"/>
-      <c r="I71" s="16" t="s">
+      <c r="H71" s="16"/>
+      <c r="I71" s="13" t="s">
         <v>268</v>
       </c>
       <c r="J71" s="6">
         <v>10</v>
       </c>
-      <c r="K71" s="13"/>
+      <c r="K71" s="16"/>
       <c r="L71" t="s">
         <v>150</v>
       </c>
@@ -3064,14 +3132,14 @@
       </c>
     </row>
     <row r="72" spans="8:13">
-      <c r="H72" s="13"/>
-      <c r="I72" s="16" t="s">
+      <c r="H72" s="16"/>
+      <c r="I72" s="17" t="s">
         <v>269</v>
       </c>
       <c r="J72" s="6">
         <v>1</v>
       </c>
-      <c r="K72" s="13"/>
+      <c r="K72" s="16"/>
       <c r="L72" t="s">
         <v>151</v>
       </c>
@@ -3080,14 +3148,14 @@
       </c>
     </row>
     <row r="73" spans="8:13">
-      <c r="H73" s="13"/>
-      <c r="I73" s="16" t="s">
+      <c r="H73" s="16"/>
+      <c r="I73" s="17" t="s">
         <v>270</v>
       </c>
       <c r="J73" s="6">
         <v>1</v>
       </c>
-      <c r="K73" s="13"/>
+      <c r="K73" s="16"/>
       <c r="L73" t="s">
         <v>152</v>
       </c>
@@ -3096,14 +3164,14 @@
       </c>
     </row>
     <row r="74" spans="8:13">
-      <c r="H74" s="13"/>
-      <c r="I74" s="16" t="s">
+      <c r="H74" s="16"/>
+      <c r="I74" s="17" t="s">
         <v>271</v>
       </c>
       <c r="J74" s="6">
         <v>1</v>
       </c>
-      <c r="K74" s="13"/>
+      <c r="K74" s="16"/>
       <c r="L74" t="s">
         <v>153</v>
       </c>
@@ -3112,14 +3180,14 @@
       </c>
     </row>
     <row r="75" spans="8:13">
-      <c r="H75" s="13"/>
-      <c r="I75" s="16" t="s">
+      <c r="H75" s="16"/>
+      <c r="I75" s="17" t="s">
         <v>272</v>
       </c>
       <c r="J75" s="6">
         <v>1</v>
       </c>
-      <c r="K75" s="13"/>
+      <c r="K75" s="16"/>
       <c r="L75" t="s">
         <v>154</v>
       </c>
@@ -3128,14 +3196,14 @@
       </c>
     </row>
     <row r="76" spans="8:13">
-      <c r="H76" s="13"/>
-      <c r="I76" s="16" t="s">
+      <c r="H76" s="16"/>
+      <c r="I76" s="17" t="s">
         <v>273</v>
       </c>
       <c r="J76" s="6">
         <v>1</v>
       </c>
-      <c r="K76" s="13"/>
+      <c r="K76" s="16"/>
       <c r="L76" t="s">
         <v>155</v>
       </c>
@@ -3144,14 +3212,14 @@
       </c>
     </row>
     <row r="77" spans="8:13">
-      <c r="H77" s="13"/>
-      <c r="I77" s="16" t="s">
+      <c r="H77" s="16"/>
+      <c r="I77" s="17" t="s">
         <v>274</v>
       </c>
       <c r="J77" s="6">
         <v>1</v>
       </c>
-      <c r="K77" s="13"/>
+      <c r="K77" s="16"/>
       <c r="L77" t="s">
         <v>156</v>
       </c>
@@ -3160,7 +3228,16 @@
       </c>
     </row>
     <row r="78" spans="8:13">
-      <c r="K78" s="13"/>
+      <c r="H78" s="16">
+        <v>45902</v>
+      </c>
+      <c r="I78" s="17" t="s">
+        <v>275</v>
+      </c>
+      <c r="J78" s="6">
+        <v>19</v>
+      </c>
+      <c r="K78" s="16"/>
       <c r="L78" t="s">
         <v>157</v>
       </c>
@@ -3169,7 +3246,14 @@
       </c>
     </row>
     <row r="79" spans="8:13">
-      <c r="K79" s="13"/>
+      <c r="H79" s="16"/>
+      <c r="I79" s="17" t="s">
+        <v>276</v>
+      </c>
+      <c r="J79" s="6">
+        <v>3</v>
+      </c>
+      <c r="K79" s="16"/>
       <c r="L79" t="s">
         <v>158</v>
       </c>
@@ -3178,7 +3262,14 @@
       </c>
     </row>
     <row r="80" spans="8:13">
-      <c r="K80" s="13"/>
+      <c r="H80" s="16"/>
+      <c r="I80" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="J80" s="6">
+        <v>10</v>
+      </c>
+      <c r="K80" s="16"/>
       <c r="L80" t="s">
         <v>159</v>
       </c>
@@ -3186,8 +3277,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="81" spans="11:13">
-      <c r="K81" s="13"/>
+    <row r="81" spans="8:13">
+      <c r="H81" s="16"/>
+      <c r="I81" s="17" t="s">
+        <v>278</v>
+      </c>
+      <c r="J81" s="6">
+        <v>16</v>
+      </c>
+      <c r="K81" s="16"/>
       <c r="L81" s="8" t="s">
         <v>160</v>
       </c>
@@ -3195,8 +3293,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="82" spans="11:13">
-      <c r="K82" s="13"/>
+    <row r="82" spans="8:13">
+      <c r="H82" s="16"/>
+      <c r="I82" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="J82" s="6">
+        <v>15</v>
+      </c>
+      <c r="K82" s="16"/>
       <c r="L82" t="s">
         <v>161</v>
       </c>
@@ -3204,8 +3309,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="83" spans="11:13">
-      <c r="K83" s="13"/>
+    <row r="83" spans="8:13">
+      <c r="H83" s="16"/>
+      <c r="I83" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="J83" s="6">
+        <v>20</v>
+      </c>
+      <c r="K83" s="16"/>
       <c r="L83" t="s">
         <v>162</v>
       </c>
@@ -3213,8 +3325,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="11:13">
-      <c r="K84" s="13"/>
+    <row r="84" spans="8:13">
+      <c r="H84" s="16"/>
+      <c r="I84" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="J84" s="6">
+        <v>8</v>
+      </c>
+      <c r="K84" s="16"/>
       <c r="L84" t="s">
         <v>163</v>
       </c>
@@ -3222,8 +3341,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="85" spans="11:13">
-      <c r="K85" s="13"/>
+    <row r="85" spans="8:13">
+      <c r="H85" s="16"/>
+      <c r="I85" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="J85" s="6">
+        <v>20</v>
+      </c>
+      <c r="K85" s="16"/>
       <c r="L85" t="s">
         <v>164</v>
       </c>
@@ -3231,8 +3357,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="86" spans="11:13">
-      <c r="K86" s="13"/>
+    <row r="86" spans="8:13">
+      <c r="H86" s="16"/>
+      <c r="I86" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="J86" s="6">
+        <v>37</v>
+      </c>
+      <c r="K86" s="16"/>
       <c r="L86" t="s">
         <v>165</v>
       </c>
@@ -3240,8 +3373,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="11:13">
-      <c r="K87" s="13"/>
+    <row r="87" spans="8:13">
+      <c r="H87" s="16"/>
+      <c r="I87" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="J87" s="6">
+        <v>6</v>
+      </c>
+      <c r="K87" s="16"/>
       <c r="L87" t="s">
         <v>166</v>
       </c>
@@ -3249,8 +3389,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="11:13">
-      <c r="K88" s="13"/>
+    <row r="88" spans="8:13">
+      <c r="H88" s="16"/>
+      <c r="I88" t="s">
+        <v>285</v>
+      </c>
+      <c r="J88" s="6">
+        <v>10</v>
+      </c>
+      <c r="K88" s="16"/>
       <c r="L88" t="s">
         <v>167</v>
       </c>
@@ -3258,8 +3405,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="11:13">
-      <c r="K89" s="13"/>
+    <row r="89" spans="8:13">
+      <c r="H89" s="16"/>
+      <c r="I89" t="s">
+        <v>286</v>
+      </c>
+      <c r="J89" s="6">
+        <v>0</v>
+      </c>
+      <c r="K89" s="16"/>
       <c r="L89" t="s">
         <v>168</v>
       </c>
@@ -3267,8 +3421,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="90" spans="11:13">
-      <c r="K90" s="13"/>
+    <row r="90" spans="8:13">
+      <c r="H90" s="16"/>
+      <c r="I90" s="17" t="s">
+        <v>287</v>
+      </c>
+      <c r="J90" s="6">
+        <v>8</v>
+      </c>
+      <c r="K90" s="16"/>
       <c r="L90" t="s">
         <v>169</v>
       </c>
@@ -3276,8 +3437,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="11:13">
-      <c r="K91" s="13"/>
+    <row r="91" spans="8:13">
+      <c r="H91" s="16"/>
+      <c r="I91" s="17" t="s">
+        <v>288</v>
+      </c>
+      <c r="J91" s="6">
+        <v>8</v>
+      </c>
+      <c r="K91" s="16"/>
       <c r="L91" t="s">
         <v>170</v>
       </c>
@@ -3285,8 +3453,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="92" spans="11:13">
-      <c r="K92" s="13"/>
+    <row r="92" spans="8:13">
+      <c r="H92" s="16"/>
+      <c r="I92" s="17" t="s">
+        <v>289</v>
+      </c>
+      <c r="J92" s="6">
+        <v>4</v>
+      </c>
+      <c r="K92" s="16"/>
       <c r="L92" t="s">
         <v>171</v>
       </c>
@@ -3294,8 +3469,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="11:13">
-      <c r="K93" s="13"/>
+    <row r="93" spans="8:13">
+      <c r="H93" s="16"/>
+      <c r="I93" s="17" t="s">
+        <v>290</v>
+      </c>
+      <c r="J93" s="6">
+        <v>8</v>
+      </c>
+      <c r="K93" s="16"/>
       <c r="L93" t="s">
         <v>172</v>
       </c>
@@ -3303,8 +3485,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="11:13">
-      <c r="K94" s="13"/>
+    <row r="94" spans="8:13">
+      <c r="H94" s="16"/>
+      <c r="I94" s="17" t="s">
+        <v>291</v>
+      </c>
+      <c r="J94" s="6">
+        <v>28</v>
+      </c>
+      <c r="K94" s="16"/>
       <c r="L94" t="s">
         <v>173</v>
       </c>
@@ -3312,8 +3501,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="95" spans="11:13">
-      <c r="K95" s="13"/>
+    <row r="95" spans="8:13">
+      <c r="H95" s="16"/>
+      <c r="I95" s="17" t="s">
+        <v>292</v>
+      </c>
+      <c r="J95" s="6">
+        <v>24</v>
+      </c>
+      <c r="K95" s="16"/>
       <c r="L95" t="s">
         <v>174</v>
       </c>
@@ -3321,8 +3517,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="96" spans="11:13">
-      <c r="K96" s="13"/>
+    <row r="96" spans="8:13">
+      <c r="K96" s="16"/>
       <c r="L96" t="s">
         <v>175</v>
       </c>
@@ -3331,7 +3527,7 @@
       </c>
     </row>
     <row r="97" spans="11:13">
-      <c r="K97" s="13"/>
+      <c r="K97" s="16"/>
       <c r="L97" t="s">
         <v>176</v>
       </c>
@@ -3340,7 +3536,7 @@
       </c>
     </row>
     <row r="98" spans="11:13">
-      <c r="K98" s="13"/>
+      <c r="K98" s="16"/>
       <c r="L98" t="s">
         <v>177</v>
       </c>
@@ -3349,7 +3545,7 @@
       </c>
     </row>
     <row r="99" spans="11:13">
-      <c r="K99" s="13"/>
+      <c r="K99" s="16"/>
       <c r="L99" t="s">
         <v>178</v>
       </c>
@@ -3358,7 +3554,7 @@
       </c>
     </row>
     <row r="100" spans="11:13">
-      <c r="K100" s="13"/>
+      <c r="K100" s="16"/>
       <c r="L100" t="s">
         <v>179</v>
       </c>
@@ -3367,7 +3563,7 @@
       </c>
     </row>
     <row r="101" spans="11:13">
-      <c r="K101" s="13"/>
+      <c r="K101" s="16"/>
       <c r="L101" t="s">
         <v>180</v>
       </c>
@@ -3376,7 +3572,7 @@
       </c>
     </row>
     <row r="102" spans="11:13">
-      <c r="K102" s="13"/>
+      <c r="K102" s="16"/>
       <c r="L102" t="s">
         <v>181</v>
       </c>
@@ -3385,7 +3581,7 @@
       </c>
     </row>
     <row r="103" spans="11:13">
-      <c r="K103" s="13"/>
+      <c r="K103" s="16"/>
       <c r="L103" t="s">
         <v>182</v>
       </c>
@@ -3394,7 +3590,7 @@
       </c>
     </row>
     <row r="104" spans="11:13">
-      <c r="K104" s="13"/>
+      <c r="K104" s="16"/>
       <c r="L104" t="s">
         <v>183</v>
       </c>
@@ -3403,7 +3599,7 @@
       </c>
     </row>
     <row r="105" spans="11:13">
-      <c r="K105" s="13"/>
+      <c r="K105" s="16"/>
       <c r="L105" t="s">
         <v>184</v>
       </c>
@@ -3412,7 +3608,7 @@
       </c>
     </row>
     <row r="106" spans="11:13">
-      <c r="K106" s="13"/>
+      <c r="K106" s="16"/>
       <c r="L106" t="s">
         <v>185</v>
       </c>
@@ -3421,7 +3617,7 @@
       </c>
     </row>
     <row r="107" spans="11:13">
-      <c r="K107" s="13"/>
+      <c r="K107" s="16"/>
       <c r="L107" t="s">
         <v>186</v>
       </c>
@@ -3430,7 +3626,7 @@
       </c>
     </row>
     <row r="108" spans="11:13">
-      <c r="K108" s="13"/>
+      <c r="K108" s="16"/>
       <c r="L108" t="s">
         <v>187</v>
       </c>
@@ -3439,7 +3635,7 @@
       </c>
     </row>
     <row r="109" spans="11:13">
-      <c r="K109" s="13"/>
+      <c r="K109" s="16"/>
       <c r="L109" t="s">
         <v>188</v>
       </c>
@@ -3448,7 +3644,7 @@
       </c>
     </row>
     <row r="110" spans="11:13">
-      <c r="K110" s="13"/>
+      <c r="K110" s="16"/>
       <c r="L110" t="s">
         <v>189</v>
       </c>
@@ -3457,7 +3653,7 @@
       </c>
     </row>
     <row r="111" spans="11:13">
-      <c r="K111" s="13"/>
+      <c r="K111" s="16"/>
       <c r="L111" t="s">
         <v>190</v>
       </c>
@@ -3466,7 +3662,7 @@
       </c>
     </row>
     <row r="112" spans="11:13">
-      <c r="K112" s="13"/>
+      <c r="K112" s="16"/>
       <c r="L112" t="s">
         <v>191</v>
       </c>
@@ -3475,7 +3671,7 @@
       </c>
     </row>
     <row r="113" spans="11:13">
-      <c r="K113" s="13"/>
+      <c r="K113" s="16"/>
       <c r="L113" t="s">
         <v>192</v>
       </c>
@@ -3484,7 +3680,7 @@
       </c>
     </row>
     <row r="114" spans="11:13">
-      <c r="K114" s="13"/>
+      <c r="K114" s="16"/>
       <c r="L114" t="s">
         <v>193</v>
       </c>
@@ -3493,7 +3689,7 @@
       </c>
     </row>
     <row r="115" spans="11:13">
-      <c r="K115" s="13"/>
+      <c r="K115" s="16"/>
       <c r="L115" t="s">
         <v>194</v>
       </c>
@@ -3502,7 +3698,7 @@
       </c>
     </row>
     <row r="116" spans="11:13">
-      <c r="K116" s="13"/>
+      <c r="K116" s="16"/>
       <c r="L116" t="s">
         <v>195</v>
       </c>
@@ -3511,7 +3707,7 @@
       </c>
     </row>
     <row r="117" spans="11:13">
-      <c r="K117" s="13"/>
+      <c r="K117" s="16"/>
       <c r="L117" t="s">
         <v>196</v>
       </c>
@@ -3520,7 +3716,7 @@
       </c>
     </row>
     <row r="118" spans="11:13">
-      <c r="K118" s="13"/>
+      <c r="K118" s="16"/>
       <c r="L118" t="s">
         <v>197</v>
       </c>
@@ -3529,7 +3725,7 @@
       </c>
     </row>
     <row r="119" spans="11:13">
-      <c r="K119" s="13"/>
+      <c r="K119" s="16"/>
       <c r="L119" t="s">
         <v>198</v>
       </c>
@@ -3538,7 +3734,7 @@
       </c>
     </row>
     <row r="120" spans="11:13">
-      <c r="K120" s="13"/>
+      <c r="K120" s="16"/>
       <c r="L120" t="s">
         <v>199</v>
       </c>
@@ -3547,7 +3743,7 @@
       </c>
     </row>
     <row r="121" spans="11:13">
-      <c r="K121" s="13"/>
+      <c r="K121" s="16"/>
       <c r="L121" t="s">
         <v>200</v>
       </c>
@@ -3556,7 +3752,7 @@
       </c>
     </row>
     <row r="122" spans="11:13">
-      <c r="K122" s="13"/>
+      <c r="K122" s="16"/>
       <c r="L122" t="s">
         <v>201</v>
       </c>
@@ -3565,7 +3761,7 @@
       </c>
     </row>
     <row r="123" spans="11:13">
-      <c r="K123" s="13"/>
+      <c r="K123" s="16"/>
       <c r="L123" t="s">
         <v>202</v>
       </c>
@@ -3574,7 +3770,7 @@
       </c>
     </row>
     <row r="124" spans="11:13">
-      <c r="K124" s="13"/>
+      <c r="K124" s="16"/>
       <c r="L124" t="s">
         <v>203</v>
       </c>
@@ -3583,7 +3779,7 @@
       </c>
     </row>
     <row r="125" spans="11:13">
-      <c r="K125" s="13"/>
+      <c r="K125" s="16"/>
       <c r="L125" t="s">
         <v>204</v>
       </c>
@@ -3592,7 +3788,7 @@
       </c>
     </row>
     <row r="126" spans="11:13">
-      <c r="K126" s="13"/>
+      <c r="K126" s="16"/>
       <c r="L126" t="s">
         <v>205</v>
       </c>
@@ -3601,7 +3797,7 @@
       </c>
     </row>
     <row r="127" spans="11:13">
-      <c r="K127" s="13"/>
+      <c r="K127" s="16"/>
       <c r="L127" t="s">
         <v>206</v>
       </c>
@@ -3610,7 +3806,7 @@
       </c>
     </row>
     <row r="128" spans="11:13">
-      <c r="K128" s="13"/>
+      <c r="K128" s="16"/>
       <c r="L128" t="s">
         <v>207</v>
       </c>
@@ -3619,7 +3815,7 @@
       </c>
     </row>
     <row r="129" spans="11:13">
-      <c r="K129" s="13"/>
+      <c r="K129" s="16"/>
       <c r="L129" t="s">
         <v>208</v>
       </c>
@@ -3628,7 +3824,7 @@
       </c>
     </row>
     <row r="130" spans="11:13">
-      <c r="K130" s="13"/>
+      <c r="K130" s="16"/>
       <c r="L130" t="s">
         <v>209</v>
       </c>
@@ -3637,7 +3833,7 @@
       </c>
     </row>
     <row r="131" spans="11:13">
-      <c r="K131" s="13"/>
+      <c r="K131" s="16"/>
       <c r="L131" t="s">
         <v>210</v>
       </c>
@@ -3646,7 +3842,7 @@
       </c>
     </row>
     <row r="132" spans="11:13">
-      <c r="K132" s="13"/>
+      <c r="K132" s="16"/>
       <c r="L132" t="s">
         <v>211</v>
       </c>
@@ -3655,7 +3851,7 @@
       </c>
     </row>
     <row r="133" spans="11:13">
-      <c r="K133" s="13"/>
+      <c r="K133" s="16"/>
       <c r="L133" t="s">
         <v>212</v>
       </c>
@@ -3664,7 +3860,7 @@
       </c>
     </row>
     <row r="134" spans="11:13">
-      <c r="K134" s="13"/>
+      <c r="K134" s="16"/>
       <c r="L134" t="s">
         <v>213</v>
       </c>
@@ -3673,7 +3869,7 @@
       </c>
     </row>
     <row r="135" spans="11:13">
-      <c r="K135" s="13"/>
+      <c r="K135" s="16"/>
       <c r="L135" t="s">
         <v>214</v>
       </c>
@@ -3682,7 +3878,7 @@
       </c>
     </row>
     <row r="136" spans="11:13">
-      <c r="K136" s="13"/>
+      <c r="K136" s="16"/>
       <c r="L136" t="s">
         <v>215</v>
       </c>
@@ -3691,7 +3887,7 @@
       </c>
     </row>
     <row r="137" spans="11:13">
-      <c r="K137" s="13"/>
+      <c r="K137" s="16"/>
       <c r="L137" t="s">
         <v>216</v>
       </c>
@@ -3700,7 +3896,7 @@
       </c>
     </row>
     <row r="138" spans="11:13">
-      <c r="K138" s="13"/>
+      <c r="K138" s="16"/>
       <c r="L138" t="s">
         <v>217</v>
       </c>
@@ -3709,7 +3905,7 @@
       </c>
     </row>
     <row r="139" spans="11:13">
-      <c r="K139" s="13"/>
+      <c r="K139" s="16"/>
       <c r="L139" t="s">
         <v>218</v>
       </c>
@@ -3718,7 +3914,7 @@
       </c>
     </row>
     <row r="140" spans="11:13">
-      <c r="K140" s="13"/>
+      <c r="K140" s="16"/>
       <c r="L140" t="s">
         <v>219</v>
       </c>
@@ -3727,7 +3923,7 @@
       </c>
     </row>
     <row r="141" spans="11:13">
-      <c r="K141" s="13"/>
+      <c r="K141" s="16"/>
       <c r="L141" t="s">
         <v>220</v>
       </c>
@@ -3736,7 +3932,7 @@
       </c>
     </row>
     <row r="142" spans="11:13">
-      <c r="K142" s="13"/>
+      <c r="K142" s="16"/>
       <c r="L142" t="s">
         <v>221</v>
       </c>
@@ -3745,7 +3941,7 @@
       </c>
     </row>
     <row r="143" spans="11:13">
-      <c r="K143" s="13"/>
+      <c r="K143" s="16"/>
       <c r="L143" t="s">
         <v>222</v>
       </c>
@@ -3754,7 +3950,7 @@
       </c>
     </row>
     <row r="144" spans="11:13">
-      <c r="K144" s="13"/>
+      <c r="K144" s="16"/>
       <c r="L144" t="s">
         <v>223</v>
       </c>
@@ -3763,7 +3959,7 @@
       </c>
     </row>
     <row r="145" spans="11:13">
-      <c r="K145" s="13"/>
+      <c r="K145" s="16"/>
       <c r="L145" t="s">
         <v>224</v>
       </c>
@@ -3772,7 +3968,7 @@
       </c>
     </row>
     <row r="146" spans="11:13">
-      <c r="K146" s="13"/>
+      <c r="K146" s="16"/>
       <c r="L146" t="s">
         <v>225</v>
       </c>
@@ -3781,7 +3977,7 @@
       </c>
     </row>
     <row r="147" spans="11:13">
-      <c r="K147" s="13"/>
+      <c r="K147" s="16"/>
       <c r="L147" t="s">
         <v>226</v>
       </c>
@@ -3790,7 +3986,14 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="K8:K44"/>
+    <mergeCell ref="K45:K147"/>
+    <mergeCell ref="H37:H54"/>
+    <mergeCell ref="H55:H65"/>
+    <mergeCell ref="H66:H77"/>
+    <mergeCell ref="H78:H95"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="E5:G5"/>
     <mergeCell ref="H5:J5"/>
@@ -3800,12 +4003,6 @@
     <mergeCell ref="B18:B34"/>
     <mergeCell ref="H21:H34"/>
     <mergeCell ref="E21:E29"/>
-    <mergeCell ref="H35:H36"/>
-    <mergeCell ref="K8:K44"/>
-    <mergeCell ref="K45:K147"/>
-    <mergeCell ref="H37:H54"/>
-    <mergeCell ref="H55:H65"/>
-    <mergeCell ref="H66:H77"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -3813,54 +4010,69 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B92F9BC-6318-413C-87D9-FEE5073A822A}">
-  <dimension ref="A2:J8"/>
+  <dimension ref="A2:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10">
-      <c r="B2" s="12" t="s">
+    <row r="2" spans="1:9">
+      <c r="B2" s="18" t="s">
         <v>248</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="18"/>
+      <c r="D2" s="18" t="s">
         <v>251</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="E2" s="18"/>
+      <c r="F2" s="18" t="s">
         <v>249</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="G2" s="18"/>
+      <c r="H2" s="18" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="I2" s="18"/>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="12" t="s">
         <v>252</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="15">
         <f>Arkusz1!D4</f>
-        <v>0.71026490066225167</v>
-      </c>
-      <c r="C3">
+        <v>0.68713294180459161</v>
+      </c>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15">
         <f>Arkusz1!G4</f>
-        <v>0.84933774834437081</v>
-      </c>
-      <c r="D3">
+        <v>0.82167645488521091</v>
+      </c>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15">
         <f>Arkusz1!J4</f>
-        <v>0.70640176600441507</v>
-      </c>
-      <c r="E3">
+        <v>0.81366791243993597</v>
+      </c>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15">
         <f>Arkusz1!M4</f>
-        <v>1.7339955849889626</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>1.6775226908702616</v>
+      </c>
+      <c r="I3" s="15"/>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3868,184 +4080,197 @@
         <f>IF((B$3*$A4)&gt;=3,"Zaliczenie","Warunek")</f>
         <v>Warunek</v>
       </c>
-      <c r="C4" t="str">
-        <f t="shared" ref="C4:E8" si="0">IF((C$3*$A4)&gt;=3,"Zaliczenie","Warunek")</f>
+      <c r="C4">
+        <f>B$3*$A4</f>
+        <v>2.0613988254137747</v>
+      </c>
+      <c r="D4" t="str">
+        <f>IF((D$3*$A4)&gt;=3,"Zaliczenie","Warunek")</f>
         <v>Warunek</v>
       </c>
-      <c r="D4" t="str">
+      <c r="E4">
+        <f>D$3*$A4</f>
+        <v>2.4650293646556327</v>
+      </c>
+      <c r="F4" t="str">
+        <f>IF((F$3*$A4)&gt;=3,"Zaliczenie","Warunek")</f>
+        <v>Warunek</v>
+      </c>
+      <c r="G4">
+        <f>F$3*$A4</f>
+        <v>2.4410037373198081</v>
+      </c>
+      <c r="H4" t="str">
+        <f>IF((H$3*$A4)&gt;=3,"Zaliczenie","Warunek")</f>
+        <v>Zaliczenie</v>
+      </c>
+      <c r="I4">
+        <f>H$3*$A4</f>
+        <v>5.0325680726107844</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5">
+        <v>3.5</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" ref="B5:B8" si="0">IF((B$3*$A5)&gt;=3,"Zaliczenie","Warunek")</f>
+        <v>Warunek</v>
+      </c>
+      <c r="C5">
+        <f>B$3*$A5</f>
+        <v>2.4049652963160706</v>
+      </c>
+      <c r="D5" t="str">
+        <f>IF((D$3*$A5)&gt;=3,"Zaliczenie","Warunek")</f>
+        <v>Warunek</v>
+      </c>
+      <c r="E5">
+        <f>D$3*$A5</f>
+        <v>2.8758675920982384</v>
+      </c>
+      <c r="F5" t="str">
+        <f>IF((F$3*$A5)&gt;=3,"Zaliczenie","Warunek")</f>
+        <v>Warunek</v>
+      </c>
+      <c r="G5">
+        <f>F$3*$A5</f>
+        <v>2.847837693539776</v>
+      </c>
+      <c r="H5" t="str">
+        <f>IF((H$3*$A5)&gt;=3,"Zaliczenie","Warunek")</f>
+        <v>Zaliczenie</v>
+      </c>
+      <c r="I5">
+        <f>H$3*$A5</f>
+        <v>5.8713294180459155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="str">
         <f t="shared" si="0"/>
         <v>Warunek</v>
       </c>
-      <c r="E4" t="str">
+      <c r="C6">
+        <f>B$3*$A6</f>
+        <v>2.7485317672183665</v>
+      </c>
+      <c r="D6" t="str">
+        <f>IF((D$3*$A6)&gt;=3,"Zaliczenie","Warunek")</f>
+        <v>Zaliczenie</v>
+      </c>
+      <c r="E6">
+        <f>D$3*$A6</f>
+        <v>3.2867058195408436</v>
+      </c>
+      <c r="F6" t="str">
+        <f>IF((F$3*$A6)&gt;=3,"Zaliczenie","Warunek")</f>
+        <v>Zaliczenie</v>
+      </c>
+      <c r="G6">
+        <f>F$3*$A6</f>
+        <v>3.2546716497597439</v>
+      </c>
+      <c r="H6" t="str">
+        <f>IF((H$3*$A6)&gt;=3,"Zaliczenie","Warunek")</f>
+        <v>Zaliczenie</v>
+      </c>
+      <c r="I6">
+        <f>H$3*$A6</f>
+        <v>6.7100907634810465</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7">
+        <v>4.5</v>
+      </c>
+      <c r="B7" t="str">
         <f t="shared" si="0"/>
         <v>Zaliczenie</v>
       </c>
-      <c r="G4">
-        <f>B$3*$A4</f>
-        <v>2.1307947019867548</v>
-      </c>
-      <c r="H4">
-        <f t="shared" ref="H4:J4" si="1">C$3*$A4</f>
-        <v>2.5480132450331126</v>
-      </c>
-      <c r="I4">
-        <f t="shared" si="1"/>
-        <v>2.1192052980132452</v>
-      </c>
-      <c r="J4">
-        <f t="shared" si="1"/>
-        <v>5.2019867549668879</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5">
-        <v>3.5</v>
-      </c>
-      <c r="B5" t="str">
-        <f t="shared" ref="B5:B8" si="2">IF((B$3*$A5)&gt;=3,"Zaliczenie","Warunek")</f>
-        <v>Warunek</v>
-      </c>
-      <c r="C5" t="str">
-        <f t="shared" si="0"/>
-        <v>Warunek</v>
-      </c>
-      <c r="D5" t="str">
-        <f t="shared" si="0"/>
-        <v>Warunek</v>
-      </c>
-      <c r="E5" t="str">
+      <c r="C7">
+        <f>B$3*$A7</f>
+        <v>3.0920982381206623</v>
+      </c>
+      <c r="D7" t="str">
+        <f>IF((D$3*$A7)&gt;=3,"Zaliczenie","Warunek")</f>
+        <v>Zaliczenie</v>
+      </c>
+      <c r="E7">
+        <f>D$3*$A7</f>
+        <v>3.6975440469834489</v>
+      </c>
+      <c r="F7" t="str">
+        <f>IF((F$3*$A7)&gt;=3,"Zaliczenie","Warunek")</f>
+        <v>Zaliczenie</v>
+      </c>
+      <c r="G7">
+        <f>F$3*$A7</f>
+        <v>3.6615056059797118</v>
+      </c>
+      <c r="H7" t="str">
+        <f>IF((H$3*$A7)&gt;=3,"Zaliczenie","Warunek")</f>
+        <v>Zaliczenie</v>
+      </c>
+      <c r="I7">
+        <f>H$3*$A7</f>
+        <v>7.5488521089161775</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="str">
         <f t="shared" si="0"/>
         <v>Zaliczenie</v>
       </c>
-      <c r="G5">
-        <f t="shared" ref="G5:G8" si="3">B$3*$A5</f>
-        <v>2.4859271523178808</v>
-      </c>
-      <c r="H5">
-        <f t="shared" ref="H5:H8" si="4">C$3*$A5</f>
-        <v>2.9726821192052979</v>
-      </c>
-      <c r="I5">
-        <f t="shared" ref="I5:I8" si="5">D$3*$A5</f>
-        <v>2.4724061810154527</v>
-      </c>
-      <c r="J5">
-        <f t="shared" ref="J5:J7" si="6">E$3*$A5</f>
-        <v>6.0689845474613691</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="str">
-        <f t="shared" si="2"/>
-        <v>Warunek</v>
-      </c>
-      <c r="C6" t="str">
-        <f t="shared" si="0"/>
+      <c r="C8">
+        <f>B$3*$A8</f>
+        <v>3.4356647090229582</v>
+      </c>
+      <c r="D8" t="str">
+        <f>IF((D$3*$A8)&gt;=3,"Zaliczenie","Warunek")</f>
         <v>Zaliczenie</v>
       </c>
-      <c r="D6" t="str">
-        <f t="shared" si="0"/>
-        <v>Warunek</v>
-      </c>
-      <c r="E6" t="str">
-        <f t="shared" si="0"/>
+      <c r="E8">
+        <f>D$3*$A8</f>
+        <v>4.1083822744260541</v>
+      </c>
+      <c r="F8" t="str">
+        <f>IF((F$3*$A8)&gt;=3,"Zaliczenie","Warunek")</f>
         <v>Zaliczenie</v>
       </c>
-      <c r="G6">
-        <f t="shared" si="3"/>
-        <v>2.8410596026490067</v>
-      </c>
-      <c r="H6">
-        <f t="shared" si="4"/>
-        <v>3.3973509933774833</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="5"/>
-        <v>2.8256070640176603</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="6"/>
-        <v>6.9359823399558502</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7">
-        <v>4.5</v>
-      </c>
-      <c r="B7" t="str">
-        <f t="shared" si="2"/>
+      <c r="G8">
+        <f>F$3*$A8</f>
+        <v>4.0683395621996796</v>
+      </c>
+      <c r="H8" t="str">
+        <f>IF((H$3*$A8)&gt;=3,"Zaliczenie","Warunek")</f>
         <v>Zaliczenie</v>
       </c>
-      <c r="C7" t="str">
-        <f t="shared" si="0"/>
-        <v>Zaliczenie</v>
-      </c>
-      <c r="D7" t="str">
-        <f t="shared" si="0"/>
-        <v>Zaliczenie</v>
-      </c>
-      <c r="E7" t="str">
-        <f t="shared" si="0"/>
-        <v>Zaliczenie</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="3"/>
-        <v>3.1961920529801326</v>
-      </c>
-      <c r="H7">
-        <f t="shared" si="4"/>
-        <v>3.8220198675496686</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="5"/>
-        <v>3.1788079470198678</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="6"/>
-        <v>7.8029801324503314</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8">
-        <v>5</v>
-      </c>
-      <c r="B8" t="str">
-        <f t="shared" si="2"/>
-        <v>Zaliczenie</v>
-      </c>
-      <c r="C8" t="str">
-        <f t="shared" si="0"/>
-        <v>Zaliczenie</v>
-      </c>
-      <c r="D8" t="str">
-        <f t="shared" si="0"/>
-        <v>Zaliczenie</v>
-      </c>
-      <c r="E8" t="str">
-        <f t="shared" si="0"/>
-        <v>Zaliczenie</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="3"/>
-        <v>3.5513245033112586</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="4"/>
-        <v>4.2466887417218544</v>
-      </c>
       <c r="I8">
-        <f t="shared" si="5"/>
-        <v>3.5320088300220753</v>
-      </c>
-      <c r="J8">
-        <f>E$3*$A8</f>
-        <v>8.6699779249448135</v>
+        <f>H$3*$A8</f>
+        <v>8.3876134543513086</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="C4:C8 D4:D8 E4:E8 G4:G8 F4:F8 H4:H8" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Aktualizacja raportu o dokumentację projektową
</commit_message>
<xml_diff>
--- a/Raport.xlsx
+++ b/Raport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\majer\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F2D5D08-DB8E-43B8-973D-462389DA1EC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A136F589-5BCA-4FB5-A27A-E86719FACBEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="274">
   <si>
     <t>Liczba członków zespołu</t>
   </si>
@@ -851,18 +851,29 @@
   </si>
   <si>
     <t>zrobione na nowo/TokyoGarden.Tests/TokyoGarden.DAL.Tests/ZamowieniaRepositoryInMemoryTests.cs</t>
+  </si>
+  <si>
+    <t>Tokyo-Garden-Restaurant/Dokumentacja projektu Tokyo Garden.docx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -960,14 +971,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -976,11 +987,14 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -992,13 +1006,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1010,8 +1021,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1503,8 +1517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C53" sqref="C52:C53"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -1541,7 +1555,7 @@
       <c r="B3" s="1"/>
       <c r="D3">
         <f>SUM(D7:D1001)</f>
-        <v>2034</v>
+        <v>2165</v>
       </c>
       <c r="G3">
         <f>SUM(G7:G1001)</f>
@@ -1563,19 +1577,19 @@
       <c r="B4" s="1"/>
       <c r="D4">
         <f>($B$2*D$3)/SUM($D$3:$AK$3)</f>
-        <v>0.95638885623604086</v>
+        <v>1.0025468858532067</v>
       </c>
       <c r="G4">
         <f>($B$2*G$3)/SUM($D$3:$AK$3)</f>
-        <v>0.72363935582461503</v>
+        <v>0.71266496874276453</v>
       </c>
       <c r="J4">
         <f>($B$2*J$3)/SUM($D$3:$AK$3)</f>
-        <v>0.84260021159045495</v>
+        <v>0.82982171799027549</v>
       </c>
       <c r="M4">
         <f>($B$2*M$3)/SUM($D$3:$AK$3)</f>
-        <v>1.477371576348889</v>
+        <v>1.4549664274137533</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -2778,7 +2792,16 @@
         <v>31</v>
       </c>
     </row>
-    <row r="49" spans="8:13">
+    <row r="49" spans="2:13">
+      <c r="B49" s="3">
+        <v>45916</v>
+      </c>
+      <c r="C49" s="18" t="s">
+        <v>273</v>
+      </c>
+      <c r="D49">
+        <v>131</v>
+      </c>
       <c r="H49" s="14"/>
       <c r="I49" s="13" t="s">
         <v>251</v>
@@ -2794,7 +2817,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="50" spans="8:13">
+    <row r="50" spans="2:13">
       <c r="H50" s="14"/>
       <c r="I50" s="13" t="s">
         <v>232</v>
@@ -2810,7 +2833,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="51" spans="8:13">
+    <row r="51" spans="2:13">
       <c r="H51" s="14"/>
       <c r="I51" s="13" t="s">
         <v>233</v>
@@ -2826,7 +2849,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="52" spans="8:13">
+    <row r="52" spans="2:13">
       <c r="H52" s="14"/>
       <c r="I52" s="13" t="s">
         <v>234</v>
@@ -2842,7 +2865,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="53" spans="8:13">
+    <row r="53" spans="2:13">
       <c r="H53" s="14"/>
       <c r="I53" s="13" t="s">
         <v>235</v>
@@ -2858,7 +2881,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="8:13">
+    <row r="54" spans="2:13">
       <c r="H54" s="14"/>
       <c r="I54" s="13" t="s">
         <v>236</v>
@@ -2874,7 +2897,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="8:13">
+    <row r="55" spans="2:13">
       <c r="H55" s="14"/>
       <c r="I55" s="13" t="s">
         <v>237</v>
@@ -2890,7 +2913,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="8:13">
+    <row r="56" spans="2:13">
       <c r="H56" s="14"/>
       <c r="I56" s="13" t="s">
         <v>238</v>
@@ -2906,7 +2929,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="8:13">
+    <row r="57" spans="2:13">
       <c r="H57" s="14"/>
       <c r="I57" s="13" t="s">
         <v>239</v>
@@ -2922,7 +2945,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="8:13">
+    <row r="58" spans="2:13">
       <c r="H58" s="14"/>
       <c r="I58" s="13" t="s">
         <v>240</v>
@@ -2938,7 +2961,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="8:13">
+    <row r="59" spans="2:13">
       <c r="H59" s="14"/>
       <c r="I59" s="13" t="s">
         <v>241</v>
@@ -2954,7 +2977,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="8:13">
+    <row r="60" spans="2:13">
       <c r="H60" s="14"/>
       <c r="I60" s="13" t="s">
         <v>242</v>
@@ -2970,7 +2993,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="61" spans="8:13">
+    <row r="61" spans="2:13">
       <c r="H61" s="14"/>
       <c r="I61" s="13" t="s">
         <v>243</v>
@@ -2986,7 +3009,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="62" spans="8:13">
+    <row r="62" spans="2:13">
       <c r="H62" s="14"/>
       <c r="I62" s="13" t="s">
         <v>244</v>
@@ -3002,7 +3025,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="63" spans="8:13">
+    <row r="63" spans="2:13">
       <c r="H63" s="14"/>
       <c r="I63" s="13" t="s">
         <v>245</v>
@@ -3018,7 +3041,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="8:13">
+    <row r="64" spans="2:13">
       <c r="H64" s="14"/>
       <c r="I64" s="13" t="s">
         <v>246</v>
@@ -4039,22 +4062,22 @@
       </c>
       <c r="B3" s="16">
         <f>Arkusz1!D4</f>
-        <v>0.95638885623604086</v>
+        <v>1.0025468858532067</v>
       </c>
       <c r="C3" s="16"/>
       <c r="D3" s="16">
         <f>Arkusz1!G4</f>
-        <v>0.72363935582461503</v>
+        <v>0.71266496874276453</v>
       </c>
       <c r="E3" s="16"/>
       <c r="F3" s="16">
         <f>Arkusz1!J4</f>
-        <v>0.84260021159045495</v>
+        <v>0.82982171799027549</v>
       </c>
       <c r="G3" s="16"/>
       <c r="H3" s="16">
         <f>Arkusz1!M4</f>
-        <v>1.477371576348889</v>
+        <v>1.4549664274137533</v>
       </c>
       <c r="I3" s="16"/>
     </row>
@@ -4064,11 +4087,11 @@
       </c>
       <c r="B4" t="str">
         <f>IF((B$3*$A4)&gt;=3,"Zaliczenie","Warunek")</f>
-        <v>Warunek</v>
+        <v>Zaliczenie</v>
       </c>
       <c r="C4">
         <f>B$3*$A4</f>
-        <v>2.8691665687081227</v>
+        <v>3.0076406575596204</v>
       </c>
       <c r="D4" t="str">
         <f>IF((D$3*$A4)&gt;=3,"Zaliczenie","Warunek")</f>
@@ -4076,7 +4099,7 @@
       </c>
       <c r="E4">
         <f>D$3*$A4</f>
-        <v>2.1709180674738451</v>
+        <v>2.1379949062282937</v>
       </c>
       <c r="F4" t="str">
         <f>IF((F$3*$A4)&gt;=3,"Zaliczenie","Warunek")</f>
@@ -4084,7 +4107,7 @@
       </c>
       <c r="G4">
         <f>F$3*$A4</f>
-        <v>2.5278006347713649</v>
+        <v>2.4894651539708263</v>
       </c>
       <c r="H4" t="str">
         <f>IF((H$3*$A4)&gt;=3,"Zaliczenie","Warunek")</f>
@@ -4092,7 +4115,7 @@
       </c>
       <c r="I4">
         <f>H$3*$A4</f>
-        <v>4.4321147290466669</v>
+        <v>4.36489928224126</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -4105,7 +4128,7 @@
       </c>
       <c r="C5">
         <f>B$3*$A5</f>
-        <v>3.3473609968261431</v>
+        <v>3.5089141004862237</v>
       </c>
       <c r="D5" t="str">
         <f>IF((D$3*$A5)&gt;=3,"Zaliczenie","Warunek")</f>
@@ -4113,7 +4136,7 @@
       </c>
       <c r="E5">
         <f>D$3*$A5</f>
-        <v>2.5327377453861528</v>
+        <v>2.4943273905996759</v>
       </c>
       <c r="F5" t="str">
         <f>IF((F$3*$A5)&gt;=3,"Zaliczenie","Warunek")</f>
@@ -4121,7 +4144,7 @@
       </c>
       <c r="G5">
         <f>F$3*$A5</f>
-        <v>2.9491007405665925</v>
+        <v>2.9043760129659644</v>
       </c>
       <c r="H5" t="str">
         <f>IF((H$3*$A5)&gt;=3,"Zaliczenie","Warunek")</f>
@@ -4129,7 +4152,7 @@
       </c>
       <c r="I5">
         <f>H$3*$A5</f>
-        <v>5.170800517221112</v>
+        <v>5.0923824959481365</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -4142,7 +4165,7 @@
       </c>
       <c r="C6">
         <f>B$3*$A6</f>
-        <v>3.8255554249441635</v>
+        <v>4.0101875434128269</v>
       </c>
       <c r="D6" t="str">
         <f>IF((D$3*$A6)&gt;=3,"Zaliczenie","Warunek")</f>
@@ -4150,7 +4173,7 @@
       </c>
       <c r="E6">
         <f>D$3*$A6</f>
-        <v>2.8945574232984601</v>
+        <v>2.8506598749710581</v>
       </c>
       <c r="F6" t="str">
         <f>IF((F$3*$A6)&gt;=3,"Zaliczenie","Warunek")</f>
@@ -4158,7 +4181,7 @@
       </c>
       <c r="G6">
         <f>F$3*$A6</f>
-        <v>3.3704008463618198</v>
+        <v>3.3192868719611019</v>
       </c>
       <c r="H6" t="str">
         <f>IF((H$3*$A6)&gt;=3,"Zaliczenie","Warunek")</f>
@@ -4166,7 +4189,7 @@
       </c>
       <c r="I6">
         <f>H$3*$A6</f>
-        <v>5.9094863053955562</v>
+        <v>5.819865709655013</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -4179,7 +4202,7 @@
       </c>
       <c r="C7">
         <f>B$3*$A7</f>
-        <v>4.3037498530621843</v>
+        <v>4.5114609863394302</v>
       </c>
       <c r="D7" t="str">
         <f>IF((D$3*$A7)&gt;=3,"Zaliczenie","Warunek")</f>
@@ -4187,7 +4210,7 @@
       </c>
       <c r="E7">
         <f>D$3*$A7</f>
-        <v>3.2563771012107674</v>
+        <v>3.2069923593424403</v>
       </c>
       <c r="F7" t="str">
         <f>IF((F$3*$A7)&gt;=3,"Zaliczenie","Warunek")</f>
@@ -4195,7 +4218,7 @@
       </c>
       <c r="G7">
         <f>F$3*$A7</f>
-        <v>3.7917009521570471</v>
+        <v>3.7341977309562395</v>
       </c>
       <c r="H7" t="str">
         <f>IF((H$3*$A7)&gt;=3,"Zaliczenie","Warunek")</f>
@@ -4203,7 +4226,7 @@
       </c>
       <c r="I7">
         <f>H$3*$A7</f>
-        <v>6.6481720935700004</v>
+        <v>6.5473489233618896</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -4216,7 +4239,7 @@
       </c>
       <c r="C8">
         <f>B$3*$A8</f>
-        <v>4.7819442811802046</v>
+        <v>5.0127344292660334</v>
       </c>
       <c r="D8" t="str">
         <f>IF((D$3*$A8)&gt;=3,"Zaliczenie","Warunek")</f>
@@ -4224,7 +4247,7 @@
       </c>
       <c r="E8">
         <f>D$3*$A8</f>
-        <v>3.6181967791230751</v>
+        <v>3.5633248437138225</v>
       </c>
       <c r="F8" t="str">
         <f>IF((F$3*$A8)&gt;=3,"Zaliczenie","Warunek")</f>
@@ -4232,7 +4255,7 @@
       </c>
       <c r="G8">
         <f>F$3*$A8</f>
-        <v>4.2130010579522743</v>
+        <v>4.1491085899513775</v>
       </c>
       <c r="H8" t="str">
         <f>IF((H$3*$A8)&gt;=3,"Zaliczenie","Warunek")</f>
@@ -4240,7 +4263,7 @@
       </c>
       <c r="I8">
         <f>H$3*$A8</f>
-        <v>7.3868578817444455</v>
+        <v>7.2748321370687661</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
poprawiona wersja dokumentacji i raportu
</commit_message>
<xml_diff>
--- a/Raport.xlsx
+++ b/Raport.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dominik\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\majer\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CDB98F2-AE72-4A17-ADE5-D0FDC754929D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37048A8F-4FBE-4B76-98B7-A2DB7E3B38D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1025,6 +1025,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1033,9 +1036,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1527,8 +1527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10:H20"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -1565,7 +1565,7 @@
       <c r="B3" s="1"/>
       <c r="D3">
         <f>SUM(D7:D1001)</f>
-        <v>2165</v>
+        <v>2254</v>
       </c>
       <c r="G3">
         <f>SUM(G7:G1001)</f>
@@ -1587,42 +1587,42 @@
       <c r="B4" s="1"/>
       <c r="D4">
         <f>($B$2*D$3)/SUM($D$3:$AK$3)</f>
-        <v>0.92383187540004263</v>
+        <v>0.95276339427242951</v>
       </c>
       <c r="G4">
         <f>($B$2*G$3)/SUM($D$3:$AK$3)</f>
-        <v>0.7924045231491359</v>
+        <v>0.78495191799640707</v>
       </c>
       <c r="J4">
         <f>($B$2*J$3)/SUM($D$3:$AK$3)</f>
-        <v>0.94303392361851934</v>
+        <v>0.93416464123428089</v>
       </c>
       <c r="M4">
         <f>($B$2*M$3)/SUM($D$3:$AK$3)</f>
-        <v>1.3407296778323021</v>
+        <v>1.3281200464968825</v>
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="17" t="s">
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17" t="s">
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17" t="s">
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
     </row>
     <row r="6" spans="1:13">
       <c r="B6" t="s">
@@ -1728,7 +1728,7 @@
       <c r="J8">
         <v>100</v>
       </c>
-      <c r="K8" s="15">
+      <c r="K8" s="16">
         <v>45772</v>
       </c>
       <c r="L8" t="s">
@@ -1739,7 +1739,7 @@
       </c>
     </row>
     <row r="9" spans="1:13">
-      <c r="B9" s="15">
+      <c r="B9" s="16">
         <v>45785</v>
       </c>
       <c r="C9" t="s">
@@ -1766,7 +1766,7 @@
       <c r="J9">
         <v>118</v>
       </c>
-      <c r="K9" s="15"/>
+      <c r="K9" s="16"/>
       <c r="L9" s="5" t="s">
         <v>17</v>
       </c>
@@ -1775,7 +1775,7 @@
       </c>
     </row>
     <row r="10" spans="1:13">
-      <c r="B10" s="15"/>
+      <c r="B10" s="16"/>
       <c r="C10" t="s">
         <v>64</v>
       </c>
@@ -1788,7 +1788,7 @@
       <c r="G10">
         <v>57</v>
       </c>
-      <c r="H10" s="15">
+      <c r="H10" s="16">
         <v>45803</v>
       </c>
       <c r="I10" t="s">
@@ -1797,7 +1797,7 @@
       <c r="J10">
         <v>70</v>
       </c>
-      <c r="K10" s="15"/>
+      <c r="K10" s="16"/>
       <c r="L10" t="s">
         <v>18</v>
       </c>
@@ -1806,7 +1806,7 @@
       </c>
     </row>
     <row r="11" spans="1:13">
-      <c r="B11" s="15"/>
+      <c r="B11" s="16"/>
       <c r="C11" t="s">
         <v>65</v>
       </c>
@@ -1819,14 +1819,14 @@
       <c r="G11">
         <v>59</v>
       </c>
-      <c r="H11" s="15"/>
+      <c r="H11" s="16"/>
       <c r="I11" t="s">
         <v>75</v>
       </c>
       <c r="J11">
         <v>23</v>
       </c>
-      <c r="K11" s="15"/>
+      <c r="K11" s="16"/>
       <c r="L11" t="s">
         <v>19</v>
       </c>
@@ -1835,7 +1835,7 @@
       </c>
     </row>
     <row r="12" spans="1:13">
-      <c r="B12" s="15"/>
+      <c r="B12" s="16"/>
       <c r="C12" t="s">
         <v>66</v>
       </c>
@@ -1848,14 +1848,14 @@
       <c r="G12">
         <v>58</v>
       </c>
-      <c r="H12" s="15"/>
+      <c r="H12" s="16"/>
       <c r="I12" t="s">
         <v>77</v>
       </c>
       <c r="J12">
         <v>23</v>
       </c>
-      <c r="K12" s="15"/>
+      <c r="K12" s="16"/>
       <c r="L12" t="s">
         <v>20</v>
       </c>
@@ -1864,7 +1864,7 @@
       </c>
     </row>
     <row r="13" spans="1:13">
-      <c r="B13" s="15"/>
+      <c r="B13" s="16"/>
       <c r="C13" t="s">
         <v>67</v>
       </c>
@@ -1877,14 +1877,14 @@
       <c r="G13">
         <v>57</v>
       </c>
-      <c r="H13" s="15"/>
+      <c r="H13" s="16"/>
       <c r="I13" t="s">
         <v>76</v>
       </c>
       <c r="J13">
         <v>27</v>
       </c>
-      <c r="K13" s="15"/>
+      <c r="K13" s="16"/>
       <c r="L13" s="5" t="s">
         <v>21</v>
       </c>
@@ -1893,7 +1893,7 @@
       </c>
     </row>
     <row r="14" spans="1:13">
-      <c r="B14" s="15"/>
+      <c r="B14" s="16"/>
       <c r="C14" t="s">
         <v>68</v>
       </c>
@@ -1906,14 +1906,14 @@
       <c r="G14">
         <v>61</v>
       </c>
-      <c r="H14" s="15"/>
+      <c r="H14" s="16"/>
       <c r="I14" t="s">
         <v>74</v>
       </c>
       <c r="J14">
         <v>24</v>
       </c>
-      <c r="K14" s="15"/>
+      <c r="K14" s="16"/>
       <c r="L14" t="s">
         <v>22</v>
       </c>
@@ -1922,7 +1922,7 @@
       </c>
     </row>
     <row r="15" spans="1:13">
-      <c r="B15" s="15"/>
+      <c r="B15" s="16"/>
       <c r="C15" t="s">
         <v>69</v>
       </c>
@@ -1935,14 +1935,14 @@
       <c r="G15">
         <v>60</v>
       </c>
-      <c r="H15" s="15"/>
+      <c r="H15" s="16"/>
       <c r="I15" t="s">
         <v>78</v>
       </c>
       <c r="J15">
         <v>27</v>
       </c>
-      <c r="K15" s="15"/>
+      <c r="K15" s="16"/>
       <c r="L15" s="5" t="s">
         <v>23</v>
       </c>
@@ -1951,7 +1951,7 @@
       </c>
     </row>
     <row r="16" spans="1:13">
-      <c r="B16" s="15"/>
+      <c r="B16" s="16"/>
       <c r="C16" t="s">
         <v>70</v>
       </c>
@@ -1964,14 +1964,14 @@
       <c r="G16">
         <v>16</v>
       </c>
-      <c r="H16" s="15"/>
+      <c r="H16" s="16"/>
       <c r="I16" t="s">
         <v>79</v>
       </c>
       <c r="J16">
         <v>27</v>
       </c>
-      <c r="K16" s="15"/>
+      <c r="K16" s="16"/>
       <c r="L16" t="s">
         <v>24</v>
       </c>
@@ -1980,7 +1980,7 @@
       </c>
     </row>
     <row r="17" spans="2:13">
-      <c r="B17" s="15"/>
+      <c r="B17" s="16"/>
       <c r="C17" t="s">
         <v>71</v>
       </c>
@@ -1993,14 +1993,14 @@
       <c r="G17">
         <v>59</v>
       </c>
-      <c r="H17" s="15"/>
+      <c r="H17" s="16"/>
       <c r="I17" t="s">
         <v>80</v>
       </c>
       <c r="J17">
         <v>27</v>
       </c>
-      <c r="K17" s="15"/>
+      <c r="K17" s="16"/>
       <c r="L17" t="s">
         <v>25</v>
       </c>
@@ -2009,7 +2009,7 @@
       </c>
     </row>
     <row r="18" spans="2:13">
-      <c r="B18" s="15">
+      <c r="B18" s="16">
         <v>45803</v>
       </c>
       <c r="C18" t="s">
@@ -2024,14 +2024,14 @@
       <c r="G18">
         <v>64</v>
       </c>
-      <c r="H18" s="15"/>
+      <c r="H18" s="16"/>
       <c r="I18" t="s">
         <v>81</v>
       </c>
       <c r="J18">
         <v>27</v>
       </c>
-      <c r="K18" s="15"/>
+      <c r="K18" s="16"/>
       <c r="L18" t="s">
         <v>26</v>
       </c>
@@ -2040,21 +2040,21 @@
       </c>
     </row>
     <row r="19" spans="2:13">
-      <c r="B19" s="15"/>
+      <c r="B19" s="16"/>
       <c r="C19" t="s">
         <v>85</v>
       </c>
       <c r="D19">
         <v>144</v>
       </c>
-      <c r="H19" s="15"/>
+      <c r="H19" s="16"/>
       <c r="I19" t="s">
         <v>82</v>
       </c>
       <c r="J19">
         <v>28</v>
       </c>
-      <c r="K19" s="15"/>
+      <c r="K19" s="16"/>
       <c r="L19" t="s">
         <v>27</v>
       </c>
@@ -2063,21 +2063,21 @@
       </c>
     </row>
     <row r="20" spans="2:13">
-      <c r="B20" s="15"/>
+      <c r="B20" s="16"/>
       <c r="C20" t="s">
         <v>86</v>
       </c>
       <c r="D20">
         <v>164</v>
       </c>
-      <c r="H20" s="15"/>
+      <c r="H20" s="16"/>
       <c r="I20" t="s">
         <v>83</v>
       </c>
       <c r="J20">
         <v>34</v>
       </c>
-      <c r="K20" s="15"/>
+      <c r="K20" s="16"/>
       <c r="L20" t="s">
         <v>28</v>
       </c>
@@ -2086,14 +2086,14 @@
       </c>
     </row>
     <row r="21" spans="2:13">
-      <c r="B21" s="15"/>
+      <c r="B21" s="16"/>
       <c r="C21" t="s">
         <v>87</v>
       </c>
       <c r="D21">
         <v>58</v>
       </c>
-      <c r="E21" s="15">
+      <c r="E21" s="16">
         <v>45804</v>
       </c>
       <c r="F21" t="s">
@@ -2102,7 +2102,7 @@
       <c r="G21">
         <v>81</v>
       </c>
-      <c r="H21" s="15">
+      <c r="H21" s="16">
         <v>45817</v>
       </c>
       <c r="I21" s="10" t="s">
@@ -2111,7 +2111,7 @@
       <c r="J21" s="6">
         <v>3</v>
       </c>
-      <c r="K21" s="15"/>
+      <c r="K21" s="16"/>
       <c r="L21" t="s">
         <v>29</v>
       </c>
@@ -2120,28 +2120,28 @@
       </c>
     </row>
     <row r="22" spans="2:13">
-      <c r="B22" s="15"/>
+      <c r="B22" s="16"/>
       <c r="C22" t="s">
         <v>88</v>
       </c>
       <c r="D22">
         <v>92</v>
       </c>
-      <c r="E22" s="17"/>
+      <c r="E22" s="18"/>
       <c r="F22" t="s">
         <v>102</v>
       </c>
       <c r="G22">
         <v>69</v>
       </c>
-      <c r="H22" s="15"/>
+      <c r="H22" s="16"/>
       <c r="I22" t="s">
         <v>111</v>
       </c>
       <c r="J22" s="6">
         <v>6</v>
       </c>
-      <c r="K22" s="15"/>
+      <c r="K22" s="16"/>
       <c r="L22" t="s">
         <v>30</v>
       </c>
@@ -2150,28 +2150,28 @@
       </c>
     </row>
     <row r="23" spans="2:13">
-      <c r="B23" s="15"/>
+      <c r="B23" s="16"/>
       <c r="C23" t="s">
         <v>89</v>
       </c>
       <c r="D23">
         <v>64</v>
       </c>
-      <c r="E23" s="17"/>
+      <c r="E23" s="18"/>
       <c r="F23" t="s">
         <v>103</v>
       </c>
       <c r="G23">
         <v>75</v>
       </c>
-      <c r="H23" s="15"/>
+      <c r="H23" s="16"/>
       <c r="I23" t="s">
         <v>112</v>
       </c>
       <c r="J23" s="6">
         <v>3</v>
       </c>
-      <c r="K23" s="15"/>
+      <c r="K23" s="16"/>
       <c r="L23" t="s">
         <v>31</v>
       </c>
@@ -2180,28 +2180,28 @@
       </c>
     </row>
     <row r="24" spans="2:13">
-      <c r="B24" s="15"/>
+      <c r="B24" s="16"/>
       <c r="C24" t="s">
         <v>90</v>
       </c>
       <c r="D24">
         <v>20</v>
       </c>
-      <c r="E24" s="17"/>
+      <c r="E24" s="18"/>
       <c r="F24" t="s">
         <v>104</v>
       </c>
       <c r="G24">
         <v>126</v>
       </c>
-      <c r="H24" s="15"/>
+      <c r="H24" s="16"/>
       <c r="I24" t="s">
         <v>113</v>
       </c>
       <c r="J24" s="6">
         <v>6</v>
       </c>
-      <c r="K24" s="15"/>
+      <c r="K24" s="16"/>
       <c r="L24" t="s">
         <v>32</v>
       </c>
@@ -2210,28 +2210,28 @@
       </c>
     </row>
     <row r="25" spans="2:13">
-      <c r="B25" s="15"/>
+      <c r="B25" s="16"/>
       <c r="C25" t="s">
         <v>91</v>
       </c>
       <c r="D25">
         <v>57</v>
       </c>
-      <c r="E25" s="17"/>
+      <c r="E25" s="18"/>
       <c r="F25" t="s">
         <v>105</v>
       </c>
       <c r="G25">
         <v>65</v>
       </c>
-      <c r="H25" s="15"/>
+      <c r="H25" s="16"/>
       <c r="I25" t="s">
         <v>114</v>
       </c>
       <c r="J25" s="6">
         <v>4</v>
       </c>
-      <c r="K25" s="15"/>
+      <c r="K25" s="16"/>
       <c r="L25" t="s">
         <v>33</v>
       </c>
@@ -2240,28 +2240,28 @@
       </c>
     </row>
     <row r="26" spans="2:13">
-      <c r="B26" s="15"/>
+      <c r="B26" s="16"/>
       <c r="C26" t="s">
         <v>92</v>
       </c>
       <c r="D26">
         <v>28</v>
       </c>
-      <c r="E26" s="17"/>
+      <c r="E26" s="18"/>
       <c r="F26" t="s">
         <v>106</v>
       </c>
       <c r="G26">
         <v>82</v>
       </c>
-      <c r="H26" s="15"/>
+      <c r="H26" s="16"/>
       <c r="I26" s="10" t="s">
         <v>115</v>
       </c>
       <c r="J26" s="6">
         <v>2</v>
       </c>
-      <c r="K26" s="15"/>
+      <c r="K26" s="16"/>
       <c r="L26" t="s">
         <v>34</v>
       </c>
@@ -2270,28 +2270,28 @@
       </c>
     </row>
     <row r="27" spans="2:13">
-      <c r="B27" s="15"/>
+      <c r="B27" s="16"/>
       <c r="C27" t="s">
         <v>93</v>
       </c>
       <c r="D27">
         <v>26</v>
       </c>
-      <c r="E27" s="17"/>
+      <c r="E27" s="18"/>
       <c r="F27" t="s">
         <v>107</v>
       </c>
       <c r="G27">
         <v>75</v>
       </c>
-      <c r="H27" s="15"/>
+      <c r="H27" s="16"/>
       <c r="I27" t="s">
         <v>116</v>
       </c>
       <c r="J27" s="6">
         <v>8</v>
       </c>
-      <c r="K27" s="15"/>
+      <c r="K27" s="16"/>
       <c r="L27" t="s">
         <v>35</v>
       </c>
@@ -2300,28 +2300,28 @@
       </c>
     </row>
     <row r="28" spans="2:13">
-      <c r="B28" s="15"/>
+      <c r="B28" s="16"/>
       <c r="C28" t="s">
         <v>94</v>
       </c>
       <c r="D28">
         <v>16</v>
       </c>
-      <c r="E28" s="17"/>
+      <c r="E28" s="18"/>
       <c r="F28" t="s">
         <v>108</v>
       </c>
       <c r="G28">
         <v>266</v>
       </c>
-      <c r="H28" s="15"/>
+      <c r="H28" s="16"/>
       <c r="I28" t="s">
         <v>117</v>
       </c>
       <c r="J28" s="6">
         <v>3</v>
       </c>
-      <c r="K28" s="15"/>
+      <c r="K28" s="16"/>
       <c r="L28" t="s">
         <v>36</v>
       </c>
@@ -2330,28 +2330,28 @@
       </c>
     </row>
     <row r="29" spans="2:13">
-      <c r="B29" s="15"/>
+      <c r="B29" s="16"/>
       <c r="C29" t="s">
         <v>95</v>
       </c>
       <c r="D29">
         <v>18</v>
       </c>
-      <c r="E29" s="17"/>
+      <c r="E29" s="18"/>
       <c r="F29" t="s">
         <v>109</v>
       </c>
       <c r="G29">
         <v>71</v>
       </c>
-      <c r="H29" s="15"/>
+      <c r="H29" s="16"/>
       <c r="I29" t="s">
         <v>118</v>
       </c>
       <c r="J29" s="6">
         <v>12</v>
       </c>
-      <c r="K29" s="15"/>
+      <c r="K29" s="16"/>
       <c r="L29" t="s">
         <v>37</v>
       </c>
@@ -2360,21 +2360,21 @@
       </c>
     </row>
     <row r="30" spans="2:13">
-      <c r="B30" s="15"/>
+      <c r="B30" s="16"/>
       <c r="C30" t="s">
         <v>96</v>
       </c>
       <c r="D30">
         <v>15</v>
       </c>
-      <c r="H30" s="15"/>
+      <c r="H30" s="16"/>
       <c r="I30" t="s">
         <v>119</v>
       </c>
       <c r="J30" s="6">
         <v>3</v>
       </c>
-      <c r="K30" s="15"/>
+      <c r="K30" s="16"/>
       <c r="L30" t="s">
         <v>38</v>
       </c>
@@ -2383,21 +2383,21 @@
       </c>
     </row>
     <row r="31" spans="2:13">
-      <c r="B31" s="15"/>
+      <c r="B31" s="16"/>
       <c r="C31" t="s">
         <v>97</v>
       </c>
       <c r="D31">
         <v>17</v>
       </c>
-      <c r="H31" s="15"/>
+      <c r="H31" s="16"/>
       <c r="I31" t="s">
         <v>120</v>
       </c>
       <c r="J31" s="6">
         <v>6</v>
       </c>
-      <c r="K31" s="15"/>
+      <c r="K31" s="16"/>
       <c r="L31" t="s">
         <v>39</v>
       </c>
@@ -2406,21 +2406,21 @@
       </c>
     </row>
     <row r="32" spans="2:13">
-      <c r="B32" s="15"/>
+      <c r="B32" s="16"/>
       <c r="C32" t="s">
         <v>98</v>
       </c>
       <c r="D32">
         <v>44</v>
       </c>
-      <c r="H32" s="15"/>
+      <c r="H32" s="16"/>
       <c r="I32" t="s">
         <v>121</v>
       </c>
       <c r="J32" s="6">
         <v>2</v>
       </c>
-      <c r="K32" s="15"/>
+      <c r="K32" s="16"/>
       <c r="L32" s="5" t="s">
         <v>40</v>
       </c>
@@ -2429,21 +2429,21 @@
       </c>
     </row>
     <row r="33" spans="2:13">
-      <c r="B33" s="15"/>
+      <c r="B33" s="16"/>
       <c r="C33" t="s">
         <v>99</v>
       </c>
       <c r="D33">
         <v>43</v>
       </c>
-      <c r="H33" s="15"/>
+      <c r="H33" s="16"/>
       <c r="I33" t="s">
         <v>122</v>
       </c>
       <c r="J33" s="6">
         <v>4</v>
       </c>
-      <c r="K33" s="15"/>
+      <c r="K33" s="16"/>
       <c r="L33" t="s">
         <v>41</v>
       </c>
@@ -2452,21 +2452,21 @@
       </c>
     </row>
     <row r="34" spans="2:13">
-      <c r="B34" s="15"/>
+      <c r="B34" s="16"/>
       <c r="C34" t="s">
         <v>100</v>
       </c>
       <c r="D34">
         <v>28</v>
       </c>
-      <c r="H34" s="15"/>
+      <c r="H34" s="16"/>
       <c r="I34" t="s">
         <v>123</v>
       </c>
       <c r="J34" s="6">
         <v>8</v>
       </c>
-      <c r="K34" s="15"/>
+      <c r="K34" s="16"/>
       <c r="L34" t="s">
         <v>42</v>
       </c>
@@ -2475,7 +2475,7 @@
       </c>
     </row>
     <row r="35" spans="2:13">
-      <c r="B35" s="15">
+      <c r="B35" s="16">
         <v>45907</v>
       </c>
       <c r="C35" t="s">
@@ -2490,7 +2490,7 @@
       <c r="G35">
         <v>300</v>
       </c>
-      <c r="H35" s="15">
+      <c r="H35" s="16">
         <v>45908</v>
       </c>
       <c r="I35" s="12" t="s">
@@ -2499,7 +2499,7 @@
       <c r="J35" s="6">
         <v>17</v>
       </c>
-      <c r="K35" s="15"/>
+      <c r="K35" s="16"/>
       <c r="L35" t="s">
         <v>43</v>
       </c>
@@ -2508,7 +2508,7 @@
       </c>
     </row>
     <row r="36" spans="2:13">
-      <c r="B36" s="17"/>
+      <c r="B36" s="18"/>
       <c r="C36" t="s">
         <v>255</v>
       </c>
@@ -2521,14 +2521,14 @@
       <c r="G36">
         <v>5</v>
       </c>
-      <c r="H36" s="15"/>
+      <c r="H36" s="16"/>
       <c r="I36" s="7" t="s">
         <v>125</v>
       </c>
       <c r="J36" s="6">
         <v>8</v>
       </c>
-      <c r="K36" s="15"/>
+      <c r="K36" s="16"/>
       <c r="L36" t="s">
         <v>44</v>
       </c>
@@ -2537,7 +2537,7 @@
       </c>
     </row>
     <row r="37" spans="2:13">
-      <c r="B37" s="17"/>
+      <c r="B37" s="18"/>
       <c r="C37" t="s">
         <v>256</v>
       </c>
@@ -2550,14 +2550,14 @@
       <c r="G37">
         <v>3</v>
       </c>
-      <c r="H37" s="15"/>
+      <c r="H37" s="16"/>
       <c r="I37" t="s">
         <v>127</v>
       </c>
       <c r="J37" s="6">
         <v>9</v>
       </c>
-      <c r="K37" s="15"/>
+      <c r="K37" s="16"/>
       <c r="L37" t="s">
         <v>45</v>
       </c>
@@ -2566,7 +2566,7 @@
       </c>
     </row>
     <row r="38" spans="2:13">
-      <c r="B38" s="17"/>
+      <c r="B38" s="18"/>
       <c r="C38" t="s">
         <v>257</v>
       </c>
@@ -2579,14 +2579,14 @@
       <c r="G38">
         <v>2</v>
       </c>
-      <c r="H38" s="15"/>
+      <c r="H38" s="16"/>
       <c r="I38" t="s">
         <v>128</v>
       </c>
       <c r="J38" s="6">
         <v>36</v>
       </c>
-      <c r="K38" s="15"/>
+      <c r="K38" s="16"/>
       <c r="L38" t="s">
         <v>46</v>
       </c>
@@ -2595,7 +2595,7 @@
       </c>
     </row>
     <row r="39" spans="2:13">
-      <c r="B39" s="17"/>
+      <c r="B39" s="18"/>
       <c r="C39" t="s">
         <v>258</v>
       </c>
@@ -2608,14 +2608,14 @@
       <c r="G39">
         <v>1</v>
       </c>
-      <c r="H39" s="15"/>
+      <c r="H39" s="16"/>
       <c r="I39" t="s">
         <v>129</v>
       </c>
       <c r="J39" s="6">
         <v>9</v>
       </c>
-      <c r="K39" s="15"/>
+      <c r="K39" s="16"/>
       <c r="L39" t="s">
         <v>47</v>
       </c>
@@ -2624,7 +2624,7 @@
       </c>
     </row>
     <row r="40" spans="2:13">
-      <c r="B40" s="17"/>
+      <c r="B40" s="18"/>
       <c r="C40" t="s">
         <v>259</v>
       </c>
@@ -2637,14 +2637,14 @@
       <c r="G40">
         <v>7</v>
       </c>
-      <c r="H40" s="15"/>
+      <c r="H40" s="16"/>
       <c r="I40" t="s">
         <v>130</v>
       </c>
       <c r="J40" s="6">
         <v>37</v>
       </c>
-      <c r="K40" s="15"/>
+      <c r="K40" s="16"/>
       <c r="L40" s="5" t="s">
         <v>48</v>
       </c>
@@ -2653,21 +2653,21 @@
       </c>
     </row>
     <row r="41" spans="2:13">
-      <c r="B41" s="17"/>
+      <c r="B41" s="18"/>
       <c r="C41" t="s">
         <v>260</v>
       </c>
       <c r="D41">
         <v>23</v>
       </c>
-      <c r="H41" s="15"/>
+      <c r="H41" s="16"/>
       <c r="I41" t="s">
         <v>131</v>
       </c>
       <c r="J41" s="6">
         <v>67</v>
       </c>
-      <c r="K41" s="15"/>
+      <c r="K41" s="16"/>
       <c r="L41" s="5" t="s">
         <v>49</v>
       </c>
@@ -2676,21 +2676,21 @@
       </c>
     </row>
     <row r="42" spans="2:13">
-      <c r="B42" s="17"/>
+      <c r="B42" s="18"/>
       <c r="C42" t="s">
         <v>261</v>
       </c>
       <c r="D42">
         <v>55</v>
       </c>
-      <c r="H42" s="15"/>
+      <c r="H42" s="16"/>
       <c r="I42" t="s">
         <v>134</v>
       </c>
       <c r="J42" s="6">
         <v>1</v>
       </c>
-      <c r="K42" s="15"/>
+      <c r="K42" s="16"/>
       <c r="L42" t="s">
         <v>50</v>
       </c>
@@ -2699,21 +2699,21 @@
       </c>
     </row>
     <row r="43" spans="2:13">
-      <c r="B43" s="17"/>
+      <c r="B43" s="18"/>
       <c r="C43" t="s">
         <v>262</v>
       </c>
       <c r="D43">
         <v>60</v>
       </c>
-      <c r="H43" s="15"/>
+      <c r="H43" s="16"/>
       <c r="I43" t="s">
         <v>139</v>
       </c>
       <c r="J43" s="6">
         <v>9</v>
       </c>
-      <c r="K43" s="15"/>
+      <c r="K43" s="16"/>
       <c r="L43" t="s">
         <v>51</v>
       </c>
@@ -2722,21 +2722,21 @@
       </c>
     </row>
     <row r="44" spans="2:13">
-      <c r="B44" s="17"/>
+      <c r="B44" s="18"/>
       <c r="C44" t="s">
         <v>263</v>
       </c>
       <c r="D44">
         <v>57</v>
       </c>
-      <c r="H44" s="15"/>
+      <c r="H44" s="16"/>
       <c r="I44" t="s">
         <v>140</v>
       </c>
       <c r="J44" s="6">
         <v>21</v>
       </c>
-      <c r="K44" s="15"/>
+      <c r="K44" s="16"/>
       <c r="L44" t="s">
         <v>52</v>
       </c>
@@ -2745,21 +2745,21 @@
       </c>
     </row>
     <row r="45" spans="2:13">
-      <c r="B45" s="17"/>
+      <c r="B45" s="18"/>
       <c r="C45" t="s">
         <v>264</v>
       </c>
       <c r="D45">
         <v>61</v>
       </c>
-      <c r="H45" s="15"/>
+      <c r="H45" s="16"/>
       <c r="I45" t="s">
         <v>147</v>
       </c>
       <c r="J45" s="6">
         <v>2</v>
       </c>
-      <c r="K45" s="15">
+      <c r="K45" s="16">
         <v>45898</v>
       </c>
       <c r="L45" s="12" t="s">
@@ -2770,21 +2770,21 @@
       </c>
     </row>
     <row r="46" spans="2:13">
-      <c r="B46" s="17"/>
+      <c r="B46" s="18"/>
       <c r="C46" t="s">
         <v>265</v>
       </c>
       <c r="D46">
         <v>69</v>
       </c>
-      <c r="H46" s="15"/>
+      <c r="H46" s="16"/>
       <c r="I46" s="13" t="s">
         <v>225</v>
       </c>
       <c r="J46" s="6">
         <v>1</v>
       </c>
-      <c r="K46" s="15"/>
+      <c r="K46" s="16"/>
       <c r="L46" s="7" t="s">
         <v>125</v>
       </c>
@@ -2793,21 +2793,21 @@
       </c>
     </row>
     <row r="47" spans="2:13">
-      <c r="B47" s="17"/>
+      <c r="B47" s="18"/>
       <c r="C47" t="s">
         <v>266</v>
       </c>
       <c r="D47">
         <v>23</v>
       </c>
-      <c r="H47" s="15"/>
+      <c r="H47" s="16"/>
       <c r="I47" s="13" t="s">
         <v>253</v>
       </c>
       <c r="J47" s="6">
         <v>15</v>
       </c>
-      <c r="K47" s="15"/>
+      <c r="K47" s="16"/>
       <c r="L47" t="s">
         <v>126</v>
       </c>
@@ -2816,21 +2816,21 @@
       </c>
     </row>
     <row r="48" spans="2:13">
-      <c r="B48" s="17"/>
+      <c r="B48" s="18"/>
       <c r="C48" t="s">
         <v>267</v>
       </c>
       <c r="D48">
         <v>55</v>
       </c>
-      <c r="H48" s="15"/>
+      <c r="H48" s="16"/>
       <c r="I48" s="13" t="s">
         <v>245</v>
       </c>
       <c r="J48" s="6">
         <v>5</v>
       </c>
-      <c r="K48" s="15"/>
+      <c r="K48" s="16"/>
       <c r="L48" t="s">
         <v>127</v>
       </c>
@@ -2846,16 +2846,16 @@
         <v>268</v>
       </c>
       <c r="D49">
-        <v>131</v>
-      </c>
-      <c r="H49" s="15"/>
+        <v>220</v>
+      </c>
+      <c r="H49" s="16"/>
       <c r="I49" s="13" t="s">
         <v>246</v>
       </c>
       <c r="J49" s="6">
         <v>5</v>
       </c>
-      <c r="K49" s="15"/>
+      <c r="K49" s="16"/>
       <c r="L49" t="s">
         <v>128</v>
       </c>
@@ -2864,14 +2864,14 @@
       </c>
     </row>
     <row r="50" spans="2:13">
-      <c r="H50" s="15"/>
+      <c r="H50" s="16"/>
       <c r="I50" s="13" t="s">
         <v>227</v>
       </c>
       <c r="J50" s="6">
         <v>45</v>
       </c>
-      <c r="K50" s="15"/>
+      <c r="K50" s="16"/>
       <c r="L50" t="s">
         <v>129</v>
       </c>
@@ -2880,14 +2880,14 @@
       </c>
     </row>
     <row r="51" spans="2:13">
-      <c r="H51" s="15"/>
+      <c r="H51" s="16"/>
       <c r="I51" s="13" t="s">
         <v>228</v>
       </c>
       <c r="J51" s="11">
         <v>24</v>
       </c>
-      <c r="K51" s="15"/>
+      <c r="K51" s="16"/>
       <c r="L51" t="s">
         <v>130</v>
       </c>
@@ -2896,14 +2896,14 @@
       </c>
     </row>
     <row r="52" spans="2:13">
-      <c r="H52" s="15"/>
+      <c r="H52" s="16"/>
       <c r="I52" s="13" t="s">
         <v>229</v>
       </c>
       <c r="J52" s="6">
         <v>26</v>
       </c>
-      <c r="K52" s="15"/>
+      <c r="K52" s="16"/>
       <c r="L52" t="s">
         <v>131</v>
       </c>
@@ -2912,14 +2912,14 @@
       </c>
     </row>
     <row r="53" spans="2:13">
-      <c r="H53" s="15"/>
+      <c r="H53" s="16"/>
       <c r="I53" s="13" t="s">
         <v>230</v>
       </c>
       <c r="J53" s="9">
         <v>1</v>
       </c>
-      <c r="K53" s="15"/>
+      <c r="K53" s="16"/>
       <c r="L53" s="8" t="s">
         <v>132</v>
       </c>
@@ -2928,14 +2928,14 @@
       </c>
     </row>
     <row r="54" spans="2:13">
-      <c r="H54" s="15"/>
+      <c r="H54" s="16"/>
       <c r="I54" s="13" t="s">
         <v>231</v>
       </c>
       <c r="J54" s="6">
         <v>18</v>
       </c>
-      <c r="K54" s="15"/>
+      <c r="K54" s="16"/>
       <c r="L54" t="s">
         <v>133</v>
       </c>
@@ -2944,14 +2944,14 @@
       </c>
     </row>
     <row r="55" spans="2:13">
-      <c r="H55" s="15"/>
+      <c r="H55" s="16"/>
       <c r="I55" s="13" t="s">
         <v>232</v>
       </c>
       <c r="J55" s="6">
         <v>1</v>
       </c>
-      <c r="K55" s="15"/>
+      <c r="K55" s="16"/>
       <c r="L55" t="s">
         <v>134</v>
       </c>
@@ -2960,14 +2960,14 @@
       </c>
     </row>
     <row r="56" spans="2:13">
-      <c r="H56" s="15"/>
+      <c r="H56" s="16"/>
       <c r="I56" s="13" t="s">
         <v>233</v>
       </c>
       <c r="J56" s="10">
         <v>32</v>
       </c>
-      <c r="K56" s="15"/>
+      <c r="K56" s="16"/>
       <c r="L56" t="s">
         <v>135</v>
       </c>
@@ -2976,14 +2976,14 @@
       </c>
     </row>
     <row r="57" spans="2:13">
-      <c r="H57" s="15"/>
+      <c r="H57" s="16"/>
       <c r="I57" s="13" t="s">
         <v>234</v>
       </c>
       <c r="J57" s="11">
         <v>1</v>
       </c>
-      <c r="K57" s="15"/>
+      <c r="K57" s="16"/>
       <c r="L57" t="s">
         <v>136</v>
       </c>
@@ -2992,14 +2992,14 @@
       </c>
     </row>
     <row r="58" spans="2:13">
-      <c r="H58" s="15"/>
+      <c r="H58" s="16"/>
       <c r="I58" s="13" t="s">
         <v>235</v>
       </c>
       <c r="J58" s="11">
         <v>18</v>
       </c>
-      <c r="K58" s="15"/>
+      <c r="K58" s="16"/>
       <c r="L58" t="s">
         <v>137</v>
       </c>
@@ -3008,14 +3008,14 @@
       </c>
     </row>
     <row r="59" spans="2:13">
-      <c r="H59" s="15"/>
+      <c r="H59" s="16"/>
       <c r="I59" s="13" t="s">
         <v>236</v>
       </c>
       <c r="J59" s="10">
         <v>1</v>
       </c>
-      <c r="K59" s="15"/>
+      <c r="K59" s="16"/>
       <c r="L59" t="s">
         <v>138</v>
       </c>
@@ -3024,14 +3024,14 @@
       </c>
     </row>
     <row r="60" spans="2:13">
-      <c r="H60" s="15"/>
+      <c r="H60" s="16"/>
       <c r="I60" s="13" t="s">
         <v>237</v>
       </c>
       <c r="J60" s="10">
         <v>14</v>
       </c>
-      <c r="K60" s="15"/>
+      <c r="K60" s="16"/>
       <c r="L60" t="s">
         <v>139</v>
       </c>
@@ -3040,14 +3040,14 @@
       </c>
     </row>
     <row r="61" spans="2:13">
-      <c r="H61" s="15"/>
+      <c r="H61" s="16"/>
       <c r="I61" s="13" t="s">
         <v>238</v>
       </c>
       <c r="J61" s="11">
         <v>2</v>
       </c>
-      <c r="K61" s="15"/>
+      <c r="K61" s="16"/>
       <c r="L61" t="s">
         <v>140</v>
       </c>
@@ -3056,14 +3056,14 @@
       </c>
     </row>
     <row r="62" spans="2:13">
-      <c r="H62" s="15"/>
+      <c r="H62" s="16"/>
       <c r="I62" s="13" t="s">
         <v>239</v>
       </c>
       <c r="J62" s="11">
         <v>17</v>
       </c>
-      <c r="K62" s="15"/>
+      <c r="K62" s="16"/>
       <c r="L62" t="s">
         <v>141</v>
       </c>
@@ -3072,14 +3072,14 @@
       </c>
     </row>
     <row r="63" spans="2:13">
-      <c r="H63" s="15"/>
+      <c r="H63" s="16"/>
       <c r="I63" s="13" t="s">
         <v>240</v>
       </c>
       <c r="J63" s="11">
         <v>1</v>
       </c>
-      <c r="K63" s="15"/>
+      <c r="K63" s="16"/>
       <c r="L63" t="s">
         <v>142</v>
       </c>
@@ -3088,14 +3088,14 @@
       </c>
     </row>
     <row r="64" spans="2:13">
-      <c r="H64" s="15"/>
+      <c r="H64" s="16"/>
       <c r="I64" s="13" t="s">
         <v>241</v>
       </c>
       <c r="J64" s="11">
         <v>12</v>
       </c>
-      <c r="K64" s="15"/>
+      <c r="K64" s="16"/>
       <c r="L64" t="s">
         <v>143</v>
       </c>
@@ -3104,14 +3104,14 @@
       </c>
     </row>
     <row r="65" spans="8:13">
-      <c r="H65" s="15"/>
+      <c r="H65" s="16"/>
       <c r="I65" s="13" t="s">
         <v>242</v>
       </c>
       <c r="J65" s="11">
         <v>43</v>
       </c>
-      <c r="K65" s="15"/>
+      <c r="K65" s="16"/>
       <c r="L65" t="s">
         <v>144</v>
       </c>
@@ -3120,14 +3120,14 @@
       </c>
     </row>
     <row r="66" spans="8:13">
-      <c r="H66" s="15"/>
+      <c r="H66" s="16"/>
       <c r="I66" s="13" t="s">
         <v>243</v>
       </c>
       <c r="J66" s="11">
         <v>53</v>
       </c>
-      <c r="K66" s="15"/>
+      <c r="K66" s="16"/>
       <c r="L66" t="s">
         <v>145</v>
       </c>
@@ -3136,14 +3136,14 @@
       </c>
     </row>
     <row r="67" spans="8:13">
-      <c r="H67" s="15"/>
+      <c r="H67" s="16"/>
       <c r="I67" s="13" t="s">
         <v>244</v>
       </c>
       <c r="J67" s="11">
         <v>66</v>
       </c>
-      <c r="K67" s="15"/>
+      <c r="K67" s="16"/>
       <c r="L67" t="s">
         <v>146</v>
       </c>
@@ -3152,14 +3152,14 @@
       </c>
     </row>
     <row r="68" spans="8:13">
-      <c r="H68" s="15"/>
+      <c r="H68" s="16"/>
       <c r="I68" s="13" t="s">
         <v>247</v>
       </c>
       <c r="J68" s="11">
         <v>13</v>
       </c>
-      <c r="K68" s="15"/>
+      <c r="K68" s="16"/>
       <c r="L68" t="s">
         <v>147</v>
       </c>
@@ -3168,14 +3168,14 @@
       </c>
     </row>
     <row r="69" spans="8:13">
-      <c r="H69" s="15"/>
+      <c r="H69" s="16"/>
       <c r="I69" s="13" t="s">
         <v>203</v>
       </c>
       <c r="J69" s="11">
         <v>10</v>
       </c>
-      <c r="K69" s="15"/>
+      <c r="K69" s="16"/>
       <c r="L69" t="s">
         <v>148</v>
       </c>
@@ -3184,14 +3184,14 @@
       </c>
     </row>
     <row r="70" spans="8:13">
-      <c r="H70" s="15"/>
+      <c r="H70" s="16"/>
       <c r="I70" s="13" t="s">
         <v>204</v>
       </c>
       <c r="J70" s="11">
         <v>40</v>
       </c>
-      <c r="K70" s="15"/>
+      <c r="K70" s="16"/>
       <c r="L70" t="s">
         <v>149</v>
       </c>
@@ -3200,14 +3200,14 @@
       </c>
     </row>
     <row r="71" spans="8:13">
-      <c r="H71" s="15"/>
+      <c r="H71" s="16"/>
       <c r="I71" s="13" t="s">
         <v>248</v>
       </c>
       <c r="J71" s="11">
         <v>15</v>
       </c>
-      <c r="K71" s="15"/>
+      <c r="K71" s="16"/>
       <c r="L71" t="s">
         <v>150</v>
       </c>
@@ -3216,14 +3216,14 @@
       </c>
     </row>
     <row r="72" spans="8:13">
-      <c r="H72" s="15"/>
+      <c r="H72" s="16"/>
       <c r="I72" s="13" t="s">
         <v>208</v>
       </c>
       <c r="J72" s="11">
         <v>8</v>
       </c>
-      <c r="K72" s="15"/>
+      <c r="K72" s="16"/>
       <c r="L72" t="s">
         <v>151</v>
       </c>
@@ -3232,14 +3232,14 @@
       </c>
     </row>
     <row r="73" spans="8:13">
-      <c r="H73" s="15"/>
+      <c r="H73" s="16"/>
       <c r="I73" s="13" t="s">
         <v>209</v>
       </c>
       <c r="J73" s="11">
         <v>19</v>
       </c>
-      <c r="K73" s="15"/>
+      <c r="K73" s="16"/>
       <c r="L73" t="s">
         <v>152</v>
       </c>
@@ -3248,14 +3248,14 @@
       </c>
     </row>
     <row r="74" spans="8:13">
-      <c r="H74" s="15"/>
+      <c r="H74" s="16"/>
       <c r="I74" s="13" t="s">
         <v>210</v>
       </c>
       <c r="J74" s="11">
         <v>14</v>
       </c>
-      <c r="K74" s="15"/>
+      <c r="K74" s="16"/>
       <c r="L74" t="s">
         <v>153</v>
       </c>
@@ -3264,14 +3264,14 @@
       </c>
     </row>
     <row r="75" spans="8:13">
-      <c r="H75" s="15"/>
+      <c r="H75" s="16"/>
       <c r="I75" t="s">
         <v>211</v>
       </c>
       <c r="J75" s="11">
         <v>2</v>
       </c>
-      <c r="K75" s="15"/>
+      <c r="K75" s="16"/>
       <c r="L75" t="s">
         <v>154</v>
       </c>
@@ -3280,14 +3280,14 @@
       </c>
     </row>
     <row r="76" spans="8:13">
-      <c r="H76" s="15"/>
+      <c r="H76" s="16"/>
       <c r="I76" t="s">
         <v>212</v>
       </c>
       <c r="J76" s="11">
         <v>22</v>
       </c>
-      <c r="K76" s="15"/>
+      <c r="K76" s="16"/>
       <c r="L76" t="s">
         <v>155</v>
       </c>
@@ -3296,14 +3296,14 @@
       </c>
     </row>
     <row r="77" spans="8:13">
-      <c r="H77" s="15"/>
+      <c r="H77" s="16"/>
       <c r="I77" s="13" t="s">
         <v>213</v>
       </c>
       <c r="J77" s="11">
         <v>11</v>
       </c>
-      <c r="K77" s="15"/>
+      <c r="K77" s="16"/>
       <c r="L77" t="s">
         <v>156</v>
       </c>
@@ -3312,14 +3312,14 @@
       </c>
     </row>
     <row r="78" spans="8:13">
-      <c r="H78" s="15"/>
+      <c r="H78" s="16"/>
       <c r="I78" t="s">
         <v>214</v>
       </c>
       <c r="J78" s="11">
         <v>9</v>
       </c>
-      <c r="K78" s="15"/>
+      <c r="K78" s="16"/>
       <c r="L78" t="s">
         <v>157</v>
       </c>
@@ -3328,14 +3328,14 @@
       </c>
     </row>
     <row r="79" spans="8:13">
-      <c r="H79" s="15"/>
+      <c r="H79" s="16"/>
       <c r="I79" t="s">
         <v>215</v>
       </c>
       <c r="J79" s="11">
         <v>33</v>
       </c>
-      <c r="K79" s="15"/>
+      <c r="K79" s="16"/>
       <c r="L79" t="s">
         <v>158</v>
       </c>
@@ -3344,14 +3344,14 @@
       </c>
     </row>
     <row r="80" spans="8:13">
-      <c r="H80" s="15"/>
+      <c r="H80" s="16"/>
       <c r="I80" s="13" t="s">
         <v>218</v>
       </c>
       <c r="J80" s="11">
         <v>15</v>
       </c>
-      <c r="K80" s="15"/>
+      <c r="K80" s="16"/>
       <c r="L80" t="s">
         <v>159</v>
       </c>
@@ -3360,14 +3360,14 @@
       </c>
     </row>
     <row r="81" spans="8:13">
-      <c r="H81" s="15"/>
+      <c r="H81" s="16"/>
       <c r="I81" s="13" t="s">
         <v>249</v>
       </c>
       <c r="J81" s="11">
         <v>7</v>
       </c>
-      <c r="K81" s="15"/>
+      <c r="K81" s="16"/>
       <c r="L81" s="8" t="s">
         <v>160</v>
       </c>
@@ -3376,14 +3376,14 @@
       </c>
     </row>
     <row r="82" spans="8:13">
-      <c r="H82" s="15"/>
+      <c r="H82" s="16"/>
       <c r="I82" s="13" t="s">
         <v>219</v>
       </c>
       <c r="J82" s="11">
         <v>12</v>
       </c>
-      <c r="K82" s="15"/>
+      <c r="K82" s="16"/>
       <c r="L82" t="s">
         <v>161</v>
       </c>
@@ -3392,14 +3392,14 @@
       </c>
     </row>
     <row r="83" spans="8:13">
-      <c r="H83" s="15"/>
+      <c r="H83" s="16"/>
       <c r="I83" s="13" t="s">
         <v>220</v>
       </c>
       <c r="J83" s="11">
         <v>107</v>
       </c>
-      <c r="K83" s="15"/>
+      <c r="K83" s="16"/>
       <c r="L83" t="s">
         <v>162</v>
       </c>
@@ -3408,14 +3408,14 @@
       </c>
     </row>
     <row r="84" spans="8:13">
-      <c r="H84" s="15"/>
+      <c r="H84" s="16"/>
       <c r="I84" s="13" t="s">
         <v>222</v>
       </c>
       <c r="J84" s="11">
         <v>12</v>
       </c>
-      <c r="K84" s="15"/>
+      <c r="K84" s="16"/>
       <c r="L84" t="s">
         <v>163</v>
       </c>
@@ -3424,14 +3424,14 @@
       </c>
     </row>
     <row r="85" spans="8:13">
-      <c r="H85" s="15"/>
+      <c r="H85" s="16"/>
       <c r="I85" t="s">
         <v>223</v>
       </c>
       <c r="J85" s="11">
         <v>6</v>
       </c>
-      <c r="K85" s="15"/>
+      <c r="K85" s="16"/>
       <c r="L85" t="s">
         <v>164</v>
       </c>
@@ -3440,14 +3440,14 @@
       </c>
     </row>
     <row r="86" spans="8:13">
-      <c r="H86" s="15"/>
+      <c r="H86" s="16"/>
       <c r="I86" s="13" t="s">
         <v>224</v>
       </c>
       <c r="J86" s="11">
         <v>24</v>
       </c>
-      <c r="K86" s="15"/>
+      <c r="K86" s="16"/>
       <c r="L86" t="s">
         <v>165</v>
       </c>
@@ -3456,14 +3456,14 @@
       </c>
     </row>
     <row r="87" spans="8:13">
-      <c r="H87" s="15"/>
+      <c r="H87" s="16"/>
       <c r="I87" s="13" t="s">
         <v>250</v>
       </c>
       <c r="J87" s="11">
         <v>64</v>
       </c>
-      <c r="K87" s="15"/>
+      <c r="K87" s="16"/>
       <c r="L87" t="s">
         <v>166</v>
       </c>
@@ -3472,14 +3472,14 @@
       </c>
     </row>
     <row r="88" spans="8:13">
-      <c r="H88" s="15"/>
+      <c r="H88" s="16"/>
       <c r="I88" s="13" t="s">
         <v>251</v>
       </c>
       <c r="J88" s="11">
         <v>38</v>
       </c>
-      <c r="K88" s="15"/>
+      <c r="K88" s="16"/>
       <c r="L88" t="s">
         <v>167</v>
       </c>
@@ -3488,14 +3488,14 @@
       </c>
     </row>
     <row r="89" spans="8:13">
-      <c r="H89" s="15"/>
+      <c r="H89" s="16"/>
       <c r="I89" s="13" t="s">
         <v>252</v>
       </c>
       <c r="J89" s="11">
         <v>42</v>
       </c>
-      <c r="K89" s="15"/>
+      <c r="K89" s="16"/>
       <c r="L89" t="s">
         <v>168</v>
       </c>
@@ -3504,14 +3504,14 @@
       </c>
     </row>
     <row r="90" spans="8:13">
-      <c r="H90" s="15"/>
+      <c r="H90" s="16"/>
       <c r="I90" t="s">
         <v>196</v>
       </c>
       <c r="J90" s="11">
         <v>2</v>
       </c>
-      <c r="K90" s="15"/>
+      <c r="K90" s="16"/>
       <c r="L90" t="s">
         <v>169</v>
       </c>
@@ -3526,10 +3526,10 @@
       <c r="I91" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="J91" s="18">
+      <c r="J91" s="15">
         <v>418</v>
       </c>
-      <c r="K91" s="15"/>
+      <c r="K91" s="16"/>
       <c r="L91" t="s">
         <v>170</v>
       </c>
@@ -3539,7 +3539,7 @@
     </row>
     <row r="92" spans="8:13">
       <c r="J92" s="6"/>
-      <c r="K92" s="15"/>
+      <c r="K92" s="16"/>
       <c r="L92" t="s">
         <v>171</v>
       </c>
@@ -3549,7 +3549,7 @@
     </row>
     <row r="93" spans="8:13">
       <c r="J93" s="6"/>
-      <c r="K93" s="15"/>
+      <c r="K93" s="16"/>
       <c r="L93" t="s">
         <v>172</v>
       </c>
@@ -3559,7 +3559,7 @@
     </row>
     <row r="94" spans="8:13">
       <c r="J94" s="6"/>
-      <c r="K94" s="15"/>
+      <c r="K94" s="16"/>
       <c r="L94" t="s">
         <v>173</v>
       </c>
@@ -3569,7 +3569,7 @@
     </row>
     <row r="95" spans="8:13">
       <c r="J95" s="6"/>
-      <c r="K95" s="15"/>
+      <c r="K95" s="16"/>
       <c r="L95" t="s">
         <v>174</v>
       </c>
@@ -3578,7 +3578,7 @@
       </c>
     </row>
     <row r="96" spans="8:13">
-      <c r="K96" s="15"/>
+      <c r="K96" s="16"/>
       <c r="L96" t="s">
         <v>175</v>
       </c>
@@ -3587,7 +3587,7 @@
       </c>
     </row>
     <row r="97" spans="11:13">
-      <c r="K97" s="15"/>
+      <c r="K97" s="16"/>
       <c r="L97" t="s">
         <v>176</v>
       </c>
@@ -3596,7 +3596,7 @@
       </c>
     </row>
     <row r="98" spans="11:13">
-      <c r="K98" s="15"/>
+      <c r="K98" s="16"/>
       <c r="L98" t="s">
         <v>177</v>
       </c>
@@ -3605,7 +3605,7 @@
       </c>
     </row>
     <row r="99" spans="11:13">
-      <c r="K99" s="15"/>
+      <c r="K99" s="16"/>
       <c r="L99" t="s">
         <v>178</v>
       </c>
@@ -3614,7 +3614,7 @@
       </c>
     </row>
     <row r="100" spans="11:13">
-      <c r="K100" s="15"/>
+      <c r="K100" s="16"/>
       <c r="L100" t="s">
         <v>179</v>
       </c>
@@ -3623,7 +3623,7 @@
       </c>
     </row>
     <row r="101" spans="11:13">
-      <c r="K101" s="15"/>
+      <c r="K101" s="16"/>
       <c r="L101" t="s">
         <v>180</v>
       </c>
@@ -3632,7 +3632,7 @@
       </c>
     </row>
     <row r="102" spans="11:13">
-      <c r="K102" s="15"/>
+      <c r="K102" s="16"/>
       <c r="L102" t="s">
         <v>181</v>
       </c>
@@ -3641,7 +3641,7 @@
       </c>
     </row>
     <row r="103" spans="11:13">
-      <c r="K103" s="15"/>
+      <c r="K103" s="16"/>
       <c r="L103" s="13" t="s">
         <v>182</v>
       </c>
@@ -3650,7 +3650,7 @@
       </c>
     </row>
     <row r="104" spans="11:13">
-      <c r="K104" s="15"/>
+      <c r="K104" s="16"/>
       <c r="L104" t="s">
         <v>183</v>
       </c>
@@ -3659,7 +3659,7 @@
       </c>
     </row>
     <row r="105" spans="11:13">
-      <c r="K105" s="15"/>
+      <c r="K105" s="16"/>
       <c r="L105" t="s">
         <v>184</v>
       </c>
@@ -3668,7 +3668,7 @@
       </c>
     </row>
     <row r="106" spans="11:13">
-      <c r="K106" s="15"/>
+      <c r="K106" s="16"/>
       <c r="L106" t="s">
         <v>185</v>
       </c>
@@ -3677,7 +3677,7 @@
       </c>
     </row>
     <row r="107" spans="11:13">
-      <c r="K107" s="15"/>
+      <c r="K107" s="16"/>
       <c r="L107" t="s">
         <v>186</v>
       </c>
@@ -3686,7 +3686,7 @@
       </c>
     </row>
     <row r="108" spans="11:13">
-      <c r="K108" s="15"/>
+      <c r="K108" s="16"/>
       <c r="L108" t="s">
         <v>187</v>
       </c>
@@ -3695,7 +3695,7 @@
       </c>
     </row>
     <row r="109" spans="11:13">
-      <c r="K109" s="15"/>
+      <c r="K109" s="16"/>
       <c r="L109" t="s">
         <v>188</v>
       </c>
@@ -3704,7 +3704,7 @@
       </c>
     </row>
     <row r="110" spans="11:13">
-      <c r="K110" s="15"/>
+      <c r="K110" s="16"/>
       <c r="L110" t="s">
         <v>189</v>
       </c>
@@ -3713,7 +3713,7 @@
       </c>
     </row>
     <row r="111" spans="11:13">
-      <c r="K111" s="15"/>
+      <c r="K111" s="16"/>
       <c r="L111" t="s">
         <v>190</v>
       </c>
@@ -3722,7 +3722,7 @@
       </c>
     </row>
     <row r="112" spans="11:13">
-      <c r="K112" s="15"/>
+      <c r="K112" s="16"/>
       <c r="L112" t="s">
         <v>191</v>
       </c>
@@ -3731,7 +3731,7 @@
       </c>
     </row>
     <row r="113" spans="11:13">
-      <c r="K113" s="15"/>
+      <c r="K113" s="16"/>
       <c r="L113" t="s">
         <v>192</v>
       </c>
@@ -3740,7 +3740,7 @@
       </c>
     </row>
     <row r="114" spans="11:13">
-      <c r="K114" s="15"/>
+      <c r="K114" s="16"/>
       <c r="L114" t="s">
         <v>193</v>
       </c>
@@ -3749,7 +3749,7 @@
       </c>
     </row>
     <row r="115" spans="11:13">
-      <c r="K115" s="15"/>
+      <c r="K115" s="16"/>
       <c r="L115" t="s">
         <v>194</v>
       </c>
@@ -3758,7 +3758,7 @@
       </c>
     </row>
     <row r="116" spans="11:13">
-      <c r="K116" s="15"/>
+      <c r="K116" s="16"/>
       <c r="L116" t="s">
         <v>195</v>
       </c>
@@ -3767,7 +3767,7 @@
       </c>
     </row>
     <row r="117" spans="11:13">
-      <c r="K117" s="15"/>
+      <c r="K117" s="16"/>
       <c r="L117" t="s">
         <v>196</v>
       </c>
@@ -3776,7 +3776,7 @@
       </c>
     </row>
     <row r="118" spans="11:13">
-      <c r="K118" s="15"/>
+      <c r="K118" s="16"/>
       <c r="L118" t="s">
         <v>197</v>
       </c>
@@ -3785,7 +3785,7 @@
       </c>
     </row>
     <row r="119" spans="11:13">
-      <c r="K119" s="15"/>
+      <c r="K119" s="16"/>
       <c r="L119" t="s">
         <v>198</v>
       </c>
@@ -3794,7 +3794,7 @@
       </c>
     </row>
     <row r="120" spans="11:13">
-      <c r="K120" s="15"/>
+      <c r="K120" s="16"/>
       <c r="L120" t="s">
         <v>199</v>
       </c>
@@ -3803,7 +3803,7 @@
       </c>
     </row>
     <row r="121" spans="11:13">
-      <c r="K121" s="15"/>
+      <c r="K121" s="16"/>
       <c r="L121" t="s">
         <v>200</v>
       </c>
@@ -3812,7 +3812,7 @@
       </c>
     </row>
     <row r="122" spans="11:13">
-      <c r="K122" s="15"/>
+      <c r="K122" s="16"/>
       <c r="L122" s="13" t="s">
         <v>201</v>
       </c>
@@ -3821,7 +3821,7 @@
       </c>
     </row>
     <row r="123" spans="11:13">
-      <c r="K123" s="15"/>
+      <c r="K123" s="16"/>
       <c r="L123" t="s">
         <v>202</v>
       </c>
@@ -3830,7 +3830,7 @@
       </c>
     </row>
     <row r="124" spans="11:13">
-      <c r="K124" s="15"/>
+      <c r="K124" s="16"/>
       <c r="L124" t="s">
         <v>203</v>
       </c>
@@ -3839,7 +3839,7 @@
       </c>
     </row>
     <row r="125" spans="11:13">
-      <c r="K125" s="15"/>
+      <c r="K125" s="16"/>
       <c r="L125" t="s">
         <v>204</v>
       </c>
@@ -3848,7 +3848,7 @@
       </c>
     </row>
     <row r="126" spans="11:13">
-      <c r="K126" s="15"/>
+      <c r="K126" s="16"/>
       <c r="L126" t="s">
         <v>205</v>
       </c>
@@ -3857,7 +3857,7 @@
       </c>
     </row>
     <row r="127" spans="11:13">
-      <c r="K127" s="15"/>
+      <c r="K127" s="16"/>
       <c r="L127" t="s">
         <v>206</v>
       </c>
@@ -3866,7 +3866,7 @@
       </c>
     </row>
     <row r="128" spans="11:13">
-      <c r="K128" s="15"/>
+      <c r="K128" s="16"/>
       <c r="L128" t="s">
         <v>207</v>
       </c>
@@ -3875,7 +3875,7 @@
       </c>
     </row>
     <row r="129" spans="11:13">
-      <c r="K129" s="15"/>
+      <c r="K129" s="16"/>
       <c r="L129" t="s">
         <v>208</v>
       </c>
@@ -3884,7 +3884,7 @@
       </c>
     </row>
     <row r="130" spans="11:13">
-      <c r="K130" s="15"/>
+      <c r="K130" s="16"/>
       <c r="L130" t="s">
         <v>209</v>
       </c>
@@ -3893,7 +3893,7 @@
       </c>
     </row>
     <row r="131" spans="11:13">
-      <c r="K131" s="15"/>
+      <c r="K131" s="16"/>
       <c r="L131" t="s">
         <v>210</v>
       </c>
@@ -3902,7 +3902,7 @@
       </c>
     </row>
     <row r="132" spans="11:13">
-      <c r="K132" s="15"/>
+      <c r="K132" s="16"/>
       <c r="L132" t="s">
         <v>211</v>
       </c>
@@ -3911,7 +3911,7 @@
       </c>
     </row>
     <row r="133" spans="11:13">
-      <c r="K133" s="15"/>
+      <c r="K133" s="16"/>
       <c r="L133" t="s">
         <v>212</v>
       </c>
@@ -3920,7 +3920,7 @@
       </c>
     </row>
     <row r="134" spans="11:13">
-      <c r="K134" s="15"/>
+      <c r="K134" s="16"/>
       <c r="L134" t="s">
         <v>213</v>
       </c>
@@ -3929,7 +3929,7 @@
       </c>
     </row>
     <row r="135" spans="11:13">
-      <c r="K135" s="15"/>
+      <c r="K135" s="16"/>
       <c r="L135" t="s">
         <v>214</v>
       </c>
@@ -3938,7 +3938,7 @@
       </c>
     </row>
     <row r="136" spans="11:13">
-      <c r="K136" s="15"/>
+      <c r="K136" s="16"/>
       <c r="L136" t="s">
         <v>215</v>
       </c>
@@ -3947,7 +3947,7 @@
       </c>
     </row>
     <row r="137" spans="11:13">
-      <c r="K137" s="15"/>
+      <c r="K137" s="16"/>
       <c r="L137" t="s">
         <v>216</v>
       </c>
@@ -3956,7 +3956,7 @@
       </c>
     </row>
     <row r="138" spans="11:13">
-      <c r="K138" s="15"/>
+      <c r="K138" s="16"/>
       <c r="L138" t="s">
         <v>217</v>
       </c>
@@ -3965,7 +3965,7 @@
       </c>
     </row>
     <row r="139" spans="11:13">
-      <c r="K139" s="15"/>
+      <c r="K139" s="16"/>
       <c r="L139" t="s">
         <v>218</v>
       </c>
@@ -3974,7 +3974,7 @@
       </c>
     </row>
     <row r="140" spans="11:13">
-      <c r="K140" s="15"/>
+      <c r="K140" s="16"/>
       <c r="L140" t="s">
         <v>219</v>
       </c>
@@ -3983,7 +3983,7 @@
       </c>
     </row>
     <row r="141" spans="11:13">
-      <c r="K141" s="15"/>
+      <c r="K141" s="16"/>
       <c r="L141" t="s">
         <v>220</v>
       </c>
@@ -3992,7 +3992,7 @@
       </c>
     </row>
     <row r="142" spans="11:13">
-      <c r="K142" s="15"/>
+      <c r="K142" s="16"/>
       <c r="L142" t="s">
         <v>221</v>
       </c>
@@ -4001,7 +4001,7 @@
       </c>
     </row>
     <row r="143" spans="11:13">
-      <c r="K143" s="15"/>
+      <c r="K143" s="16"/>
       <c r="L143" t="s">
         <v>222</v>
       </c>
@@ -4010,7 +4010,7 @@
       </c>
     </row>
     <row r="144" spans="11:13">
-      <c r="K144" s="15"/>
+      <c r="K144" s="16"/>
       <c r="L144" t="s">
         <v>223</v>
       </c>
@@ -4019,7 +4019,7 @@
       </c>
     </row>
     <row r="145" spans="11:13">
-      <c r="K145" s="15"/>
+      <c r="K145" s="16"/>
       <c r="L145" t="s">
         <v>224</v>
       </c>
@@ -4028,7 +4028,7 @@
       </c>
     </row>
     <row r="146" spans="11:13">
-      <c r="K146" s="15"/>
+      <c r="K146" s="16"/>
       <c r="L146" s="13" t="s">
         <v>225</v>
       </c>
@@ -4037,7 +4037,7 @@
       </c>
     </row>
     <row r="147" spans="11:13">
-      <c r="K147" s="15"/>
+      <c r="K147" s="16"/>
       <c r="L147" t="s">
         <v>226</v>
       </c>

</xml_diff>